<commit_message>
update vaccine efficacy according to delta variant
</commit_message>
<xml_diff>
--- a/data/vaccine/vaccine_efficacy.xlsx
+++ b/data/vaccine/vaccine_efficacy.xlsx
@@ -1,21 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Jeongjoo)\JJ_YJ shared folder\data\for code\vaccine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dropbox (Jeongjoo)\estimation_matlab\Covid19_seoul_gyeonggi\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5906CB-D6BF-41F3-84C0-E4D0AEF6F19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95679DDC-0841-4072-ACF5-8693DC9F1487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15126" yWindow="2317" windowWidth="13173" windowHeight="12772" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="776" yWindow="3181" windowWidth="15765" windowHeight="12772" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1525,8 +1534,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C321"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="G311" sqref="G311"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="18.2" x14ac:dyDescent="0.4"/>
@@ -1561,10 +1570,10 @@
       <c r="A3" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B3">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="1">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C3" s="1">
         <v>0.84099999999999997</v>
       </c>
     </row>
@@ -1572,10 +1581,10 @@
       <c r="A4" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B4">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="1">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C4" s="1">
         <v>0.84099999999999997</v>
       </c>
     </row>
@@ -1583,10 +1592,10 @@
       <c r="A5" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B5">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="1">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C5" s="1">
         <v>0.84099999999999997</v>
       </c>
     </row>
@@ -1594,10 +1603,10 @@
       <c r="A6" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B6">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="1">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C6" s="1">
         <v>0.84099999999999997</v>
       </c>
     </row>
@@ -1605,10 +1614,10 @@
       <c r="A7" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B7">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="C7">
+      <c r="B7" s="1">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C7" s="1">
         <v>0.84099999999999997</v>
       </c>
     </row>
@@ -1616,10 +1625,10 @@
       <c r="A8" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B8">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="C8">
+      <c r="B8" s="1">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C8" s="1">
         <v>0.84099999999999997</v>
       </c>
     </row>
@@ -1627,10 +1636,10 @@
       <c r="A9" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B9">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="C9">
+      <c r="B9" s="1">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C9" s="1">
         <v>0.84099999999999997</v>
       </c>
     </row>
@@ -1638,10 +1647,10 @@
       <c r="A10" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B10">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="1">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C10" s="1">
         <v>0.84099999999999997</v>
       </c>
     </row>
@@ -1649,10 +1658,10 @@
       <c r="A11" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B11">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="C11">
+      <c r="B11" s="1">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C11" s="1">
         <v>0.84099999999999997</v>
       </c>
     </row>
@@ -1660,10 +1669,10 @@
       <c r="A12" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B12">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="C12">
+      <c r="B12" s="1">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C12" s="1">
         <v>0.84099999999999997</v>
       </c>
     </row>
@@ -1671,10 +1680,10 @@
       <c r="A13" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="B13">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="C13">
+      <c r="B13" s="1">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C13" s="1">
         <v>0.84099999999999997</v>
       </c>
     </row>
@@ -1682,10 +1691,10 @@
       <c r="A14" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B14">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="C14">
+      <c r="B14" s="1">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C14" s="1">
         <v>0.84099999999999997</v>
       </c>
     </row>
@@ -1693,10 +1702,10 @@
       <c r="A15" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="B15">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="C15">
+      <c r="B15" s="1">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C15" s="1">
         <v>0.84099999999999997</v>
       </c>
     </row>
@@ -1704,10 +1713,10 @@
       <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B16">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="C16">
+      <c r="B16" s="1">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C16" s="1">
         <v>0.84099999999999997</v>
       </c>
     </row>
@@ -2717,10 +2726,10 @@
         <v>164</v>
       </c>
       <c r="B108" s="1">
-        <v>0.47380899999999992</v>
+        <v>0.47732799999999997</v>
       </c>
       <c r="C108" s="1">
-        <v>0.83789800000000003</v>
+        <v>0.83941599999999994</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.4">
@@ -2728,10 +2737,10 @@
         <v>165</v>
       </c>
       <c r="B109" s="1">
-        <v>0.47380899999999992</v>
+        <v>0.47732799999999997</v>
       </c>
       <c r="C109" s="1">
-        <v>0.83789800000000003</v>
+        <v>0.83941599999999994</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.4">
@@ -2739,10 +2748,10 @@
         <v>159</v>
       </c>
       <c r="B110" s="1">
-        <v>0.47380899999999992</v>
+        <v>0.47732799999999997</v>
       </c>
       <c r="C110" s="1">
-        <v>0.83789800000000003</v>
+        <v>0.83941599999999994</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.4">
@@ -2750,10 +2759,10 @@
         <v>157</v>
       </c>
       <c r="B111" s="1">
-        <v>0.47380899999999992</v>
+        <v>0.47732799999999997</v>
       </c>
       <c r="C111" s="1">
-        <v>0.83789800000000003</v>
+        <v>0.83941599999999994</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.4">
@@ -2761,10 +2770,10 @@
         <v>161</v>
       </c>
       <c r="B112" s="1">
-        <v>0.47380899999999992</v>
+        <v>0.47732799999999997</v>
       </c>
       <c r="C112" s="1">
-        <v>0.83789800000000003</v>
+        <v>0.83941599999999994</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.4">
@@ -2772,10 +2781,10 @@
         <v>158</v>
       </c>
       <c r="B113" s="1">
-        <v>0.47671599999999997</v>
+        <v>0.47774194752186588</v>
       </c>
       <c r="C113" s="1">
-        <v>0.83915200000000001</v>
+        <v>0.83959456559766765</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.4">
@@ -2783,10 +2792,10 @@
         <v>95</v>
       </c>
       <c r="B114" s="1">
-        <v>0.47671599999999997</v>
+        <v>0.47808853935860057</v>
       </c>
       <c r="C114" s="1">
-        <v>0.83915200000000001</v>
+        <v>0.83974407580174915</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.4">
@@ -2794,10 +2803,10 @@
         <v>180</v>
       </c>
       <c r="B115" s="1">
-        <v>0.47671599999999997</v>
+        <v>0.47836911370262392</v>
       </c>
       <c r="C115" s="1">
-        <v>0.83915200000000001</v>
+        <v>0.83986510787172008</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.4">
@@ -2805,10 +2814,10 @@
         <v>93</v>
       </c>
       <c r="B116" s="1">
-        <v>0.47671599999999997</v>
+        <v>0.47858500874635562</v>
       </c>
       <c r="C116" s="1">
-        <v>0.83915200000000001</v>
+        <v>0.83995823906705536</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.4">
@@ -2816,10 +2825,10 @@
         <v>178</v>
       </c>
       <c r="B117" s="1">
-        <v>0.47671599999999997</v>
+        <v>0.47873756268221573</v>
       </c>
       <c r="C117" s="1">
-        <v>0.83915200000000001</v>
+        <v>0.84002404664723029</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.4">
@@ -2827,10 +2836,10 @@
         <v>182</v>
       </c>
       <c r="B118" s="1">
-        <v>0.47671599999999997</v>
+        <v>0.4788281137026239</v>
       </c>
       <c r="C118" s="1">
-        <v>0.83915200000000001</v>
+        <v>0.84006310787172012</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.4">
@@ -2838,10 +2847,10 @@
         <v>172</v>
       </c>
       <c r="B119" s="1">
-        <v>0.47671599999999997</v>
+        <v>0.47885799999999995</v>
       </c>
       <c r="C119" s="1">
-        <v>0.83915200000000001</v>
+        <v>0.84007599999999993</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.4">
@@ -2849,10 +2858,10 @@
         <v>183</v>
       </c>
       <c r="B120" s="1">
-        <v>0.47549199999999997</v>
+        <v>0.47878956437010894</v>
       </c>
       <c r="C120" s="1">
-        <v>0.83862399999999993</v>
+        <v>0.84004647874789007</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.4">
@@ -2860,10 +2869,10 @@
         <v>171</v>
       </c>
       <c r="B121" s="1">
-        <v>0.47549199999999997</v>
+        <v>0.47860698327451279</v>
       </c>
       <c r="C121" s="1">
-        <v>0.83862399999999993</v>
+        <v>0.83996771827528005</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.4">
@@ -2871,10 +2880,10 @@
         <v>176</v>
       </c>
       <c r="B122" s="1">
-        <v>0.47549199999999997</v>
+        <v>0.47834434540432713</v>
       </c>
       <c r="C122" s="1">
-        <v>0.83862399999999993</v>
+        <v>0.83985442350774886</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.4">
@@ -2882,10 +2891,10 @@
         <v>174</v>
       </c>
       <c r="B123" s="1">
-        <v>0.47549199999999997</v>
+        <v>0.47803573945066752</v>
       </c>
       <c r="C123" s="1">
-        <v>0.83862399999999993</v>
+        <v>0.83972129937087614</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.4">
@@ -2893,10 +2902,10 @@
         <v>184</v>
       </c>
       <c r="B124" s="1">
-        <v>0.47549199999999997</v>
+        <v>0.47771525410464938</v>
       </c>
       <c r="C124" s="1">
-        <v>0.83862399999999993</v>
+        <v>0.83958305079024098</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.4">
@@ -2904,10 +2913,10 @@
         <v>96</v>
       </c>
       <c r="B125" s="1">
-        <v>0.47549199999999997</v>
+        <v>0.47741697805738836</v>
       </c>
       <c r="C125" s="1">
-        <v>0.83862399999999993</v>
+        <v>0.83945438269142236</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.4">
@@ -2915,10 +2924,10 @@
         <v>181</v>
       </c>
       <c r="B126" s="1">
-        <v>0.47549199999999997</v>
+        <v>0.47717499999999996</v>
       </c>
       <c r="C126" s="1">
-        <v>0.83862399999999993</v>
+        <v>0.83934999999999993</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.4">
@@ -2926,10 +2935,10 @@
         <v>185</v>
       </c>
       <c r="B127" s="1">
-        <v>0.47411499999999995</v>
+        <v>0.47699664033359734</v>
       </c>
       <c r="C127" s="1">
-        <v>0.83802999999999994</v>
+        <v>0.83927306053606165</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.4">
@@ -2937,10 +2946,10 @@
         <v>92</v>
       </c>
       <c r="B128" s="1">
-        <v>0.47411499999999995</v>
+        <v>0.47685305209659556</v>
       </c>
       <c r="C128" s="1">
-        <v>0.83802999999999994</v>
+        <v>0.83921112051225688</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.4">
@@ -2948,10 +2957,10 @@
         <v>175</v>
       </c>
       <c r="B129" s="1">
-        <v>0.47411499999999995</v>
+        <v>0.47672407293606328</v>
       </c>
       <c r="C129" s="1">
-        <v>0.83802999999999994</v>
+        <v>0.83915548244300764</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.4">
@@ -2959,10 +2968,10 @@
         <v>106</v>
       </c>
       <c r="B130" s="1">
-        <v>0.47411499999999995</v>
+        <v>0.47658954049906893</v>
       </c>
       <c r="C130" s="1">
-        <v>0.83802999999999994</v>
+        <v>0.83909744884273563</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.4">
@@ -2970,10 +2979,10 @@
         <v>99</v>
       </c>
       <c r="B131" s="1">
-        <v>0.47411499999999995</v>
+        <v>0.47642929243268123</v>
       </c>
       <c r="C131" s="1">
-        <v>0.83802999999999994</v>
+        <v>0.83902832222586243</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.4">
@@ -2981,10 +2990,10 @@
         <v>104</v>
       </c>
       <c r="B132" s="1">
-        <v>0.47411499999999995</v>
+        <v>0.47622316638396872</v>
       </c>
       <c r="C132" s="1">
-        <v>0.83802999999999994</v>
+        <v>0.83893940510681009</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.4">
@@ -2992,10 +3001,10 @@
         <v>102</v>
       </c>
       <c r="B133" s="1">
-        <v>0.47411499999999995</v>
+        <v>0.47595099999999996</v>
       </c>
       <c r="C133" s="1">
-        <v>0.83802999999999994</v>
+        <v>0.83882199999999996</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.4">
@@ -3003,10 +3012,10 @@
         <v>107</v>
       </c>
       <c r="B134" s="1">
-        <v>0.46156900000000001</v>
+        <v>0.47539917863367742</v>
       </c>
       <c r="C134" s="1">
-        <v>0.83261799999999997</v>
+        <v>0.83858395941060593</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.4">
@@ -3014,10 +3023,10 @@
         <v>103</v>
       </c>
       <c r="B135" s="1">
-        <v>0.46156900000000001</v>
+        <v>0.47441978959892833</v>
       </c>
       <c r="C135" s="1">
-        <v>0.83261799999999997</v>
+        <v>0.83816147786620443</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.4">
@@ -3025,10 +3034,10 @@
         <v>98</v>
       </c>
       <c r="B136" s="1">
-        <v>0.46156900000000001</v>
+        <v>0.47309122348435895</v>
       </c>
       <c r="C136" s="1">
-        <v>0.83261799999999997</v>
+        <v>0.83758837091482152</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.4">
@@ -3036,10 +3045,10 @@
         <v>120</v>
       </c>
       <c r="B137" s="1">
-        <v>0.46156900000000001</v>
+        <v>0.47149187087857536</v>
       </c>
       <c r="C137" s="1">
-        <v>0.83261799999999997</v>
+        <v>0.83689845410448349</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.4">
@@ -3047,10 +3056,10 @@
         <v>94</v>
       </c>
       <c r="B138" s="1">
-        <v>0.46156900000000001</v>
+        <v>0.4697001223701836</v>
       </c>
       <c r="C138" s="1">
-        <v>0.83261799999999997</v>
+        <v>0.8361255429832164</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.4">
@@ -3058,10 +3067,10 @@
         <v>115</v>
       </c>
       <c r="B139" s="1">
-        <v>0.46156900000000001</v>
+        <v>0.46779436854778977</v>
       </c>
       <c r="C139" s="1">
-        <v>0.83261799999999997</v>
+        <v>0.83530345309904652</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.4">
@@ -3069,10 +3078,10 @@
         <v>118</v>
       </c>
       <c r="B140" s="1">
-        <v>0.46156900000000001</v>
+        <v>0.46585300000000002</v>
       </c>
       <c r="C140" s="1">
-        <v>0.83261799999999997</v>
+        <v>0.83446600000000004</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.4">
@@ -3080,10 +3089,10 @@
         <v>101</v>
       </c>
       <c r="B141" s="1">
-        <v>0.44045499999999999</v>
+        <v>0.4636139186005831</v>
       </c>
       <c r="C141" s="1">
-        <v>0.82350999999999996</v>
+        <v>0.83350012174927124</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.4">
@@ -3091,10 +3100,10 @@
         <v>100</v>
       </c>
       <c r="B142" s="1">
-        <v>0.44045499999999999</v>
+        <v>0.46087195043731777</v>
       </c>
       <c r="C142" s="1">
-        <v>0.82350999999999996</v>
+        <v>0.83231731195335279</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.4">
@@ -3102,10 +3111,10 @@
         <v>119</v>
       </c>
       <c r="B143" s="1">
-        <v>0.44045499999999999</v>
+        <v>0.45779087241982502</v>
       </c>
       <c r="C143" s="1">
-        <v>0.82350999999999996</v>
+        <v>0.8309882194752185</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.4">
@@ -3113,10 +3122,10 @@
         <v>105</v>
       </c>
       <c r="B144" s="1">
-        <v>0.44045499999999999</v>
+        <v>0.45453446145772597</v>
       </c>
       <c r="C144" s="1">
-        <v>0.82350999999999996</v>
+        <v>0.82958349317784252</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.4">
@@ -3124,10 +3133,10 @@
         <v>97</v>
       </c>
       <c r="B145" s="1">
-        <v>0.44045499999999999</v>
+        <v>0.45126649446064138</v>
       </c>
       <c r="C145" s="1">
-        <v>0.82350999999999996</v>
+        <v>0.82817378192419822</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.4">
@@ -3135,10 +3144,10 @@
         <v>114</v>
       </c>
       <c r="B146" s="1">
-        <v>0.44045499999999999</v>
+        <v>0.44815074833819235</v>
       </c>
       <c r="C146" s="1">
-        <v>0.82350999999999996</v>
+        <v>0.8268297345772595</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.4">
@@ -3146,10 +3155,10 @@
         <v>137</v>
       </c>
       <c r="B147" s="1">
-        <v>0.44045499999999999</v>
+        <v>0.445351</v>
       </c>
       <c r="C147" s="1">
-        <v>0.82350999999999996</v>
+        <v>0.82562200000000008</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.4">
@@ -3157,10 +3166,10 @@
         <v>122</v>
       </c>
       <c r="B148" s="1">
-        <v>0.43858663461538461</v>
+        <v>0.44287575505246635</v>
       </c>
       <c r="C148" s="1">
-        <v>0.82270403846153839</v>
+        <v>0.82455424727753457</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.4">
@@ -3168,10 +3177,10 @@
         <v>123</v>
       </c>
       <c r="B149" s="1">
-        <v>0.43671826923076923</v>
+        <v>0.44057546922250684</v>
       </c>
       <c r="C149" s="1">
-        <v>0.82189807692307693</v>
+        <v>0.82356196711559126</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.4">
@@ -3179,10 +3188,10 @@
         <v>133</v>
       </c>
       <c r="B150" s="1">
-        <v>0.43484990384615385</v>
+        <v>0.43837684460051224</v>
       </c>
       <c r="C150" s="1">
-        <v>0.82109211538461546</v>
+        <v>0.82261354080806404</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.4">
@@ -3190,10 +3199,10 @@
         <v>113</v>
       </c>
       <c r="B151" s="1">
-        <v>0.43298153846153842</v>
+        <v>0.43620658327687345</v>
       </c>
       <c r="C151" s="1">
-        <v>0.82028615384615389</v>
+        <v>0.82167734964884731</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.4">
@@ -3201,10 +3210,10 @@
         <v>108</v>
       </c>
       <c r="B152" s="1">
-        <v>0.4311131730769231</v>
+        <v>0.43399138734198128</v>
       </c>
       <c r="C152" s="1">
-        <v>0.81948019230769231</v>
+        <v>0.82072177493183507</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.4">
@@ -3212,10 +3221,10 @@
         <v>111</v>
       </c>
       <c r="B153" s="1">
-        <v>0.42924480769230766</v>
+        <v>0.43165795888622654</v>
       </c>
       <c r="C153" s="1">
-        <v>0.81867423076923074</v>
+        <v>0.81971519795092129</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.4">
@@ -3223,10 +3232,10 @@
         <v>121</v>
       </c>
       <c r="B154" s="1">
-        <v>0.42737644230769234</v>
+        <v>0.42913299999999999</v>
       </c>
       <c r="C154" s="1">
-        <v>0.81786826923076927</v>
+        <v>0.81862599999999996</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.4">
@@ -3234,10 +3243,10 @@
         <v>110</v>
       </c>
       <c r="B155" s="1">
-        <v>0.42550807692307691</v>
+        <v>0.4263637802695599</v>
       </c>
       <c r="C155" s="1">
-        <v>0.81706230769230781</v>
+        <v>0.8174314346260847</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.4">
@@ -3245,10 +3254,10 @@
         <v>112</v>
       </c>
       <c r="B156" s="1">
-        <v>0.42363971153846153</v>
+        <v>0.42338755270111661</v>
       </c>
       <c r="C156" s="1">
-        <v>0.81625634615384612</v>
+        <v>0.81614757175342278</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.4">
@@ -3256,10 +3265,10 @@
         <v>116</v>
       </c>
       <c r="B157" s="1">
-        <v>0.42177134615384615</v>
+        <v>0.42026599451498858</v>
       </c>
       <c r="C157" s="1">
-        <v>0.81545038461538466</v>
+        <v>0.8148010172417598</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.4">
@@ -3267,10 +3276,10 @@
         <v>117</v>
       </c>
       <c r="B158" s="1">
-        <v>0.41990298076923077</v>
+        <v>0.41706078293149429</v>
       </c>
       <c r="C158" s="1">
-        <v>0.81464442307692297</v>
+        <v>0.81341837695084074</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.4">
@@ -3278,10 +3287,10 @@
         <v>109</v>
       </c>
       <c r="B159" s="1">
-        <v>0.41803461538461539</v>
+        <v>0.41383359517095242</v>
       </c>
       <c r="C159" s="1">
-        <v>0.81383846153846151</v>
+        <v>0.81202625674041085</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.4">
@@ -3289,10 +3298,10 @@
         <v>132</v>
       </c>
       <c r="B160" s="1">
-        <v>0.41616625000000002</v>
+        <v>0.41064610845368144</v>
       </c>
       <c r="C160" s="1">
-        <v>0.81303250000000005</v>
+        <v>0.81065126247021557</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.4">
@@ -3300,10 +3309,10 @@
         <v>131</v>
       </c>
       <c r="B161" s="1">
-        <v>0.41429788461538464</v>
+        <v>0.40755999999999998</v>
       </c>
       <c r="C161" s="1">
-        <v>0.81222653846153847</v>
+        <v>0.80932000000000004</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.4">
@@ -3311,10 +3320,10 @@
         <v>206</v>
       </c>
       <c r="B162" s="1">
-        <v>0.41242951923076926</v>
+        <v>0.40453480776097028</v>
       </c>
       <c r="C162" s="1">
-        <v>0.8114205769230769</v>
+        <v>0.80801501511257534</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.4">
@@ -3322,10 +3331,10 @@
         <v>65</v>
       </c>
       <c r="B163" s="1">
-        <v>0.41056115384615388</v>
+        <v>0.40150194867380518</v>
       </c>
       <c r="C163" s="1">
-        <v>0.81061461538461543</v>
+        <v>0.8067067229573277</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.4">
@@ -3333,10 +3342,10 @@
         <v>207</v>
       </c>
       <c r="B164" s="1">
-        <v>0.40869278846153845</v>
+        <v>0.398480918438049</v>
       </c>
       <c r="C164" s="1">
-        <v>0.80980865384615386</v>
+        <v>0.80540353344386428</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.4">
@@ -3344,10 +3353,10 @@
         <v>71</v>
       </c>
       <c r="B165" s="1">
-        <v>0.40682442307692313</v>
+        <v>0.39549121275324606</v>
       </c>
       <c r="C165" s="1">
-        <v>0.80900269230769228</v>
+        <v>0.80411385648179245</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.4">
@@ -3355,10 +3364,10 @@
         <v>82</v>
       </c>
       <c r="B166" s="1">
-        <v>0.40495605769230769</v>
+        <v>0.39255232731894074</v>
       </c>
       <c r="C166" s="1">
-        <v>0.80819673076923082</v>
+        <v>0.8028461019807196</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.4">
@@ -3366,10 +3375,10 @@
         <v>215</v>
       </c>
       <c r="B167" s="1">
-        <v>0.40308769230769237</v>
+        <v>0.38968375783467724</v>
       </c>
       <c r="C167" s="1">
-        <v>0.80739076923076925</v>
+        <v>0.80160867985025286</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.4">
@@ -3377,10 +3386,10 @@
         <v>76</v>
       </c>
       <c r="B168" s="1">
-        <v>0.40121932692307694</v>
+        <v>0.38690499999999994</v>
       </c>
       <c r="C168" s="1">
-        <v>0.80658480769230767</v>
+        <v>0.80041000000000007</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.4">
@@ -3388,10 +3397,10 @@
         <v>68</v>
       </c>
       <c r="B169" s="1">
-        <v>0.39935096153846161</v>
+        <v>0.38423639213906557</v>
       </c>
       <c r="C169" s="1">
-        <v>0.80577884615384621</v>
+        <v>0.79925883582469492</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.4">
@@ -3399,10 +3408,10 @@
         <v>192</v>
       </c>
       <c r="B170" s="1">
-        <v>0.39748259615384618</v>
+        <v>0.38166439028061017</v>
       </c>
       <c r="C170" s="1">
-        <v>0.80497288461538463</v>
+        <v>0.7981493448269299</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.4">
@@ -3410,10 +3419,10 @@
         <v>210</v>
       </c>
       <c r="B171" s="1">
-        <v>0.3956142307692308</v>
+        <v>0.37915766668104756</v>
       </c>
       <c r="C171" s="1">
-        <v>0.80416692307692306</v>
+        <v>0.79706801307809894</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.4">
@@ -3421,10 +3430,10 @@
         <v>193</v>
       </c>
       <c r="B172" s="1">
-        <v>0.39374586538461542</v>
+        <v>0.37668489359679147</v>
       </c>
       <c r="C172" s="1">
-        <v>0.80336096153846159</v>
+        <v>0.79600132664959633</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.4">
@@ -3432,10 +3441,10 @@
         <v>198</v>
       </c>
       <c r="B173" s="1">
-        <v>0.39187750000000005</v>
+        <v>0.37421474328425575</v>
       </c>
       <c r="C173" s="1">
-        <v>0.80255500000000002</v>
+        <v>0.79493577161281626</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.4">
@@ -3443,10 +3452,10 @@
         <v>199</v>
       </c>
       <c r="B174" s="1">
-        <v>0.39000913461538467</v>
+        <v>0.37171588799985389</v>
       </c>
       <c r="C174" s="1">
-        <v>0.80174903846153844</v>
+        <v>0.79385783403915267</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.4">
@@ -3454,10 +3463,10 @@
         <v>216</v>
       </c>
       <c r="B175" s="1">
-        <v>0.38814076923076929</v>
+        <v>0.36915699999999996</v>
       </c>
       <c r="C175" s="1">
-        <v>0.80094307692307698</v>
+        <v>0.79275400000000007</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.4">
@@ -3465,10 +3474,10 @@
         <v>200</v>
       </c>
       <c r="B176" s="1">
-        <v>0.38627240384615391</v>
+        <v>0.36638348467683912</v>
       </c>
       <c r="C176" s="1">
-        <v>0.8001371153846154</v>
+        <v>0.79155758162530321</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.4">
@@ -3476,10 +3485,10 @@
         <v>190</v>
       </c>
       <c r="B177" s="1">
-        <v>0.38440403846153853</v>
+        <v>0.3633713425088031</v>
       </c>
       <c r="C177" s="1">
-        <v>0.79933115384615383</v>
+        <v>0.79025822618026798</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.4">
@@ -3487,10 +3496,10 @@
         <v>61</v>
       </c>
       <c r="B178" s="1">
-        <v>0.38253567307692316</v>
+        <v>0.36028513838173482</v>
       </c>
       <c r="C178" s="1">
-        <v>0.79852519230769237</v>
+        <v>0.78892692243917972</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.4">
@@ -3498,10 +3507,10 @@
         <v>186</v>
       </c>
       <c r="B179" s="1">
-        <v>0.38066730769230772</v>
+        <v>0.35728943718147738</v>
       </c>
       <c r="C179" s="1">
-        <v>0.79771923076923079</v>
+        <v>0.78763465917632358</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.4">
@@ -3509,10 +3518,10 @@
         <v>195</v>
       </c>
       <c r="B180" s="1">
-        <v>0.3787989423076924</v>
+        <v>0.35454880379387371</v>
       </c>
       <c r="C180" s="1">
-        <v>0.79691326923076922</v>
+        <v>0.78645242516598479</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.4">
@@ -3520,10 +3529,10 @@
         <v>62</v>
       </c>
       <c r="B181" s="1">
-        <v>0.37693057692307697</v>
+        <v>0.35222780310476692</v>
       </c>
       <c r="C181" s="1">
-        <v>0.79610730769230775</v>
+        <v>0.7854512091824486</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.4">
@@ -3531,10 +3540,10 @@
         <v>204</v>
       </c>
       <c r="B182" s="1">
-        <v>0.37506221153846164</v>
+        <v>0.350491</v>
       </c>
       <c r="C182" s="1">
-        <v>0.79530134615384629</v>
+        <v>0.78470200000000001</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.4">
@@ -3542,10 +3551,10 @@
         <v>209</v>
       </c>
       <c r="B183" s="1">
-        <v>0.37319384615384621</v>
+        <v>0.34922565120593685</v>
       </c>
       <c r="C183" s="1">
-        <v>0.7944953846153846</v>
+        <v>0.78415616326530613</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.4">
@@ -3553,10 +3562,10 @@
         <v>197</v>
       </c>
       <c r="B184" s="1">
-        <v>0.37132548076923089</v>
+        <v>0.34816915955473093</v>
       </c>
       <c r="C184" s="1">
-        <v>0.79368942307692314</v>
+        <v>0.78370042176870758</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.4">
@@ -3564,10 +3573,10 @@
         <v>213</v>
       </c>
       <c r="B185" s="1">
-        <v>0.36945711538461545</v>
+        <v>0.34726130909090902</v>
       </c>
       <c r="C185" s="1">
-        <v>0.79288346153846156</v>
+        <v>0.78330880000000003</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.4">
@@ -3575,10 +3584,10 @@
         <v>202</v>
       </c>
       <c r="B186" s="1">
-        <v>0.36758875000000008</v>
+        <v>0.3464418838589981</v>
       </c>
       <c r="C186" s="1">
-        <v>0.7920775000000001</v>
+        <v>0.78295532244897958</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.4">
@@ -3586,10 +3595,10 @@
         <v>208</v>
       </c>
       <c r="B187" s="1">
-        <v>0.3657203846153847</v>
+        <v>0.34565066790352506</v>
       </c>
       <c r="C187" s="1">
-        <v>0.79127153846153853</v>
+        <v>0.78261401360544225</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.4">
@@ -3597,10 +3606,10 @@
         <v>212</v>
       </c>
       <c r="B188" s="1">
-        <v>0.36385201923076937</v>
+        <v>0.34482744526901665</v>
       </c>
       <c r="C188" s="1">
-        <v>0.79046557692307695</v>
+        <v>0.78225889795918369</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.4">
@@ -3608,10 +3617,10 @@
         <v>211</v>
       </c>
       <c r="B189" s="1">
-        <v>0.36198365384615394</v>
+        <v>0.343912</v>
       </c>
       <c r="C189" s="1">
-        <v>0.78965961538461549</v>
+        <v>0.781864</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.4">
@@ -3619,10 +3628,10 @@
         <v>214</v>
       </c>
       <c r="B190" s="1">
-        <v>0.36011528846153856</v>
+        <v>0.34288426098810176</v>
       </c>
       <c r="C190" s="1">
-        <v>0.78885365384615391</v>
+        <v>0.78142066160271062</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.4">
@@ -3630,10 +3639,10 @@
         <v>205</v>
       </c>
       <c r="B191" s="1">
-        <v>0.35824692307692318</v>
+        <v>0.34179069308959104</v>
       </c>
       <c r="C191" s="1">
-        <v>0.78804769230769234</v>
+        <v>0.78094892643080405</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.4">
@@ -3641,10 +3650,10 @@
         <v>43</v>
       </c>
       <c r="B192" s="1">
-        <v>0.35637855769230781</v>
+        <v>0.34067088429595771</v>
       </c>
       <c r="C192" s="1">
-        <v>0.78724173076923076</v>
+        <v>0.78046587165707992</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.4">
@@ -3652,10 +3661,10 @@
         <v>35</v>
       </c>
       <c r="B193" s="1">
-        <v>0.35451019230769243</v>
+        <v>0.33956442259869196</v>
       </c>
       <c r="C193" s="1">
-        <v>0.7864357692307693</v>
+        <v>0.77998857445433767</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.4">
@@ -3663,10 +3672,10 @@
         <v>44</v>
       </c>
       <c r="B194" s="1">
-        <v>0.35264182692307705</v>
+        <v>0.33851089598928374</v>
       </c>
       <c r="C194" s="1">
-        <v>0.78562980769230784</v>
+        <v>0.77953411199537725</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.4">
@@ -3674,10 +3683,10 @@
         <v>39</v>
       </c>
       <c r="B195" s="1">
-        <v>0.35077346153846162</v>
+        <v>0.33754989245922307</v>
       </c>
       <c r="C195" s="1">
-        <v>0.78482384615384615</v>
+        <v>0.77911956145299821</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.4">
@@ -3685,10 +3694,10 @@
         <v>45</v>
       </c>
       <c r="B196" s="1">
-        <v>0.34890509615384629</v>
+        <v>0.33672099999999999</v>
       </c>
       <c r="C196" s="1">
-        <v>0.78401788461538469</v>
+        <v>0.77876199999999995</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.4">
@@ -3696,10 +3705,10 @@
         <v>46</v>
       </c>
       <c r="B197" s="1">
-        <v>0.34703673076923086</v>
+        <v>0.33598691103931916</v>
       </c>
       <c r="C197" s="1">
-        <v>0.78321192307692322</v>
+        <v>0.778445334173824</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.4">
@@ -3707,10 +3716,10 @@
         <v>51</v>
       </c>
       <c r="B198" s="1">
-        <v>0.34516836538461548</v>
+        <v>0.33528874832558503</v>
       </c>
       <c r="C198" s="1">
-        <v>0.78240596153846165</v>
+        <v>0.77814416594437008</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.4">
@@ -3718,10 +3727,10 @@
         <v>50</v>
       </c>
       <c r="B199" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33463374533133711</v>
       </c>
       <c r="C199" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77786161563312584</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.4">
@@ -3729,10 +3738,10 @@
         <v>4</v>
       </c>
       <c r="B200" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33402913552911512</v>
       </c>
       <c r="C200" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77760080356157901</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.4">
@@ -3740,10 +3749,10 @@
         <v>201</v>
       </c>
       <c r="B201" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33348215239145851</v>
       </c>
       <c r="C201" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77736485005121747</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.4">
@@ -3751,10 +3760,10 @@
         <v>189</v>
       </c>
       <c r="B202" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33300002939090689</v>
       </c>
       <c r="C202" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77715687542352851</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.4">
@@ -3762,10 +3771,10 @@
         <v>194</v>
       </c>
       <c r="B203" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C203" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.4">
@@ -3773,10 +3782,10 @@
         <v>14</v>
       </c>
       <c r="B204" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C204" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.4">
@@ -3784,10 +3793,10 @@
         <v>8</v>
       </c>
       <c r="B205" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C205" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.4">
@@ -3795,10 +3804,10 @@
         <v>7</v>
       </c>
       <c r="B206" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C206" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.4">
@@ -3806,10 +3815,10 @@
         <v>12</v>
       </c>
       <c r="B207" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C207" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.4">
@@ -3817,10 +3826,10 @@
         <v>13</v>
       </c>
       <c r="B208" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C208" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.4">
@@ -3828,10 +3837,10 @@
         <v>188</v>
       </c>
       <c r="B209" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C209" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.4">
@@ -3839,10 +3848,10 @@
         <v>196</v>
       </c>
       <c r="B210" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C210" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.4">
@@ -3850,10 +3859,10 @@
         <v>2</v>
       </c>
       <c r="B211" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C211" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.4">
@@ -3861,10 +3870,10 @@
         <v>191</v>
       </c>
       <c r="B212" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C212" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.4">
@@ -3872,10 +3881,10 @@
         <v>187</v>
       </c>
       <c r="B213" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C213" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.4">
@@ -3883,10 +3892,10 @@
         <v>1</v>
       </c>
       <c r="B214" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C214" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.4">
@@ -3894,10 +3903,10 @@
         <v>3</v>
       </c>
       <c r="B215" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C215" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.4">
@@ -3905,10 +3914,10 @@
         <v>55</v>
       </c>
       <c r="B216" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C216" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.4">
@@ -3916,10 +3925,10 @@
         <v>57</v>
       </c>
       <c r="B217" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C217" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.4">
@@ -3927,10 +3936,10 @@
         <v>11</v>
       </c>
       <c r="B218" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C218" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.4">
@@ -3938,10 +3947,10 @@
         <v>9</v>
       </c>
       <c r="B219" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C219" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.4">
@@ -3949,10 +3958,10 @@
         <v>47</v>
       </c>
       <c r="B220" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C220" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.4">
@@ -3960,10 +3969,10 @@
         <v>60</v>
       </c>
       <c r="B221" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C221" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.4">
@@ -3971,10 +3980,10 @@
         <v>10</v>
       </c>
       <c r="B222" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C222" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.4">
@@ -3982,10 +3991,10 @@
         <v>52</v>
       </c>
       <c r="B223" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C223" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.4">
@@ -3993,10 +4002,10 @@
         <v>59</v>
       </c>
       <c r="B224" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C224" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.4">
@@ -4004,10 +4013,10 @@
         <v>49</v>
       </c>
       <c r="B225" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C225" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.4">
@@ -4015,10 +4024,10 @@
         <v>48</v>
       </c>
       <c r="B226" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C226" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.4">
@@ -4026,10 +4035,10 @@
         <v>5</v>
       </c>
       <c r="B227" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C227" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.4">
@@ -4037,10 +4046,10 @@
         <v>6</v>
       </c>
       <c r="B228" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C228" s="1">
-        <v>0.78159999999999996</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.4">
@@ -4048,10 +4057,10 @@
         <v>203</v>
       </c>
       <c r="B229" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C229" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.4">
@@ -4059,10 +4068,10 @@
         <v>231</v>
       </c>
       <c r="B230" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C230" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.4">
@@ -4070,10 +4079,10 @@
         <v>232</v>
       </c>
       <c r="B231" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C231" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.4">
@@ -4081,10 +4090,10 @@
         <v>233</v>
       </c>
       <c r="B232" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C232" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.4">
@@ -4092,10 +4101,10 @@
         <v>234</v>
       </c>
       <c r="B233" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C233" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.4">
@@ -4103,10 +4112,10 @@
         <v>235</v>
       </c>
       <c r="B234" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C234" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.4">
@@ -4114,10 +4123,10 @@
         <v>236</v>
       </c>
       <c r="B235" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C235" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.4">
@@ -4125,10 +4134,10 @@
         <v>237</v>
       </c>
       <c r="B236" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C236" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.4">
@@ -4136,10 +4145,10 @@
         <v>238</v>
       </c>
       <c r="B237" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C237" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.4">
@@ -4147,10 +4156,10 @@
         <v>239</v>
       </c>
       <c r="B238" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C238" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.4">
@@ -4158,10 +4167,10 @@
         <v>240</v>
       </c>
       <c r="B239" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C239" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.4">
@@ -4169,10 +4178,10 @@
         <v>241</v>
       </c>
       <c r="B240" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C240" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.4">
@@ -4180,10 +4189,10 @@
         <v>242</v>
       </c>
       <c r="B241" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C241" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.4">
@@ -4191,10 +4200,10 @@
         <v>243</v>
       </c>
       <c r="B242" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C242" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.4">
@@ -4202,10 +4211,10 @@
         <v>244</v>
       </c>
       <c r="B243" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C243" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.4">
@@ -4213,10 +4222,10 @@
         <v>245</v>
       </c>
       <c r="B244" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C244" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.4">
@@ -4224,10 +4233,10 @@
         <v>246</v>
       </c>
       <c r="B245" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C245" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.4">
@@ -4235,10 +4244,10 @@
         <v>247</v>
       </c>
       <c r="B246" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C246" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.4">
@@ -4246,10 +4255,10 @@
         <v>248</v>
       </c>
       <c r="B247" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C247" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.4">
@@ -4257,10 +4266,10 @@
         <v>249</v>
       </c>
       <c r="B248" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C248" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.4">
@@ -4268,10 +4277,10 @@
         <v>250</v>
       </c>
       <c r="B249" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C249" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.4">
@@ -4279,10 +4288,10 @@
         <v>251</v>
       </c>
       <c r="B250" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C250" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.4">
@@ -4290,10 +4299,10 @@
         <v>252</v>
       </c>
       <c r="B251" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C251" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.4">
@@ -4301,10 +4310,10 @@
         <v>253</v>
       </c>
       <c r="B252" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C252" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.4">
@@ -4312,10 +4321,10 @@
         <v>254</v>
       </c>
       <c r="B253" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C253" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.4">
@@ -4323,10 +4332,10 @@
         <v>255</v>
       </c>
       <c r="B254" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C254" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.4">
@@ -4334,10 +4343,10 @@
         <v>256</v>
       </c>
       <c r="B255" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C255" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.4">
@@ -4345,10 +4354,10 @@
         <v>257</v>
       </c>
       <c r="B256" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C256" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.4">
@@ -4356,10 +4365,10 @@
         <v>258</v>
       </c>
       <c r="B257" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C257" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.4">
@@ -4367,10 +4376,10 @@
         <v>259</v>
       </c>
       <c r="B258" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C258" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.4">
@@ -4378,10 +4387,10 @@
         <v>260</v>
       </c>
       <c r="B259" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C259" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.4">
@@ -4389,10 +4398,10 @@
         <v>261</v>
       </c>
       <c r="B260" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C260" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.4">
@@ -4400,10 +4409,10 @@
         <v>262</v>
       </c>
       <c r="B261" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C261" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.4">
@@ -4411,10 +4420,10 @@
         <v>263</v>
       </c>
       <c r="B262" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C262" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.4">
@@ -4422,10 +4431,10 @@
         <v>264</v>
       </c>
       <c r="B263" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C263" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.4">
@@ -4433,10 +4442,10 @@
         <v>265</v>
       </c>
       <c r="B264" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C264" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.4">
@@ -4444,10 +4453,10 @@
         <v>266</v>
       </c>
       <c r="B265" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C265" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.4">
@@ -4455,10 +4464,10 @@
         <v>267</v>
       </c>
       <c r="B266" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C266" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.4">
@@ -4466,10 +4475,10 @@
         <v>268</v>
       </c>
       <c r="B267" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C267" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.4">
@@ -4477,10 +4486,10 @@
         <v>269</v>
       </c>
       <c r="B268" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C268" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.4">
@@ -4488,10 +4497,10 @@
         <v>270</v>
       </c>
       <c r="B269" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C269" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.4">
@@ -4499,10 +4508,10 @@
         <v>271</v>
       </c>
       <c r="B270" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C270" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.4">
@@ -4510,10 +4519,10 @@
         <v>272</v>
       </c>
       <c r="B271" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C271" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.4">
@@ -4521,10 +4530,10 @@
         <v>273</v>
       </c>
       <c r="B272" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C272" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.4">
@@ -4532,10 +4541,10 @@
         <v>274</v>
       </c>
       <c r="B273" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C273" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.4">
@@ -4543,10 +4552,10 @@
         <v>275</v>
       </c>
       <c r="B274" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C274" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.4">
@@ -4554,10 +4563,10 @@
         <v>276</v>
       </c>
       <c r="B275" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C275" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.4">
@@ -4565,10 +4574,10 @@
         <v>277</v>
       </c>
       <c r="B276" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C276" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.4">
@@ -4576,10 +4585,10 @@
         <v>278</v>
       </c>
       <c r="B277" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C277" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.4">
@@ -4587,10 +4596,10 @@
         <v>279</v>
       </c>
       <c r="B278" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C278" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.4">
@@ -4598,10 +4607,10 @@
         <v>280</v>
       </c>
       <c r="B279" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C279" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.4">
@@ -4609,10 +4618,10 @@
         <v>281</v>
       </c>
       <c r="B280" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C280" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.4">
@@ -4620,10 +4629,10 @@
         <v>282</v>
       </c>
       <c r="B281" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C281" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.4">
@@ -4631,10 +4640,10 @@
         <v>283</v>
       </c>
       <c r="B282" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C282" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.4">
@@ -4642,10 +4651,10 @@
         <v>284</v>
       </c>
       <c r="B283" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C283" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.4">
@@ -4653,10 +4662,10 @@
         <v>285</v>
       </c>
       <c r="B284" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C284" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.4">
@@ -4664,10 +4673,10 @@
         <v>286</v>
       </c>
       <c r="B285" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C285" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.4">
@@ -4675,10 +4684,10 @@
         <v>287</v>
       </c>
       <c r="B286" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C286" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.4">
@@ -4686,10 +4695,10 @@
         <v>288</v>
       </c>
       <c r="B287" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C287" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.4">
@@ -4697,10 +4706,10 @@
         <v>289</v>
       </c>
       <c r="B288" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C288" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.4">
@@ -4708,10 +4717,10 @@
         <v>290</v>
       </c>
       <c r="B289" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C289" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.4">
@@ -4719,10 +4728,10 @@
         <v>291</v>
       </c>
       <c r="B290" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C290" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.4">
@@ -4730,10 +4739,10 @@
         <v>292</v>
       </c>
       <c r="B291" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C291" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.4">
@@ -4741,10 +4750,10 @@
         <v>293</v>
       </c>
       <c r="B292" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C292" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.4">
@@ -4752,10 +4761,10 @@
         <v>294</v>
       </c>
       <c r="B293" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C293" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.4">
@@ -4763,10 +4772,10 @@
         <v>295</v>
       </c>
       <c r="B294" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C294" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.4">
@@ -4774,10 +4783,10 @@
         <v>296</v>
       </c>
       <c r="B295" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C295" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.4">
@@ -4785,10 +4794,10 @@
         <v>297</v>
       </c>
       <c r="B296" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C296" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.4">
@@ -4796,10 +4805,10 @@
         <v>298</v>
       </c>
       <c r="B297" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C297" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.4">
@@ -4807,10 +4816,10 @@
         <v>299</v>
       </c>
       <c r="B298" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C298" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.4">
@@ -4818,10 +4827,10 @@
         <v>300</v>
       </c>
       <c r="B299" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C299" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.4">
@@ -4829,10 +4838,10 @@
         <v>301</v>
       </c>
       <c r="B300" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C300" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.4">
@@ -4840,10 +4849,10 @@
         <v>302</v>
       </c>
       <c r="B301" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C301" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.4">
@@ -4851,10 +4860,10 @@
         <v>303</v>
       </c>
       <c r="B302" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C302" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.4">
@@ -4862,10 +4871,10 @@
         <v>304</v>
       </c>
       <c r="B303" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C303" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.4">
@@ -4873,10 +4882,10 @@
         <v>305</v>
       </c>
       <c r="B304" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C304" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.4">
@@ -4884,10 +4893,10 @@
         <v>306</v>
       </c>
       <c r="B305" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C305" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.4">
@@ -4895,10 +4904,10 @@
         <v>307</v>
       </c>
       <c r="B306" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C306" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.4">
@@ -4906,10 +4915,10 @@
         <v>308</v>
       </c>
       <c r="B307" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C307" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.4">
@@ -4917,10 +4926,10 @@
         <v>309</v>
       </c>
       <c r="B308" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C308" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.4">
@@ -4928,10 +4937,10 @@
         <v>310</v>
       </c>
       <c r="B309" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C309" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.4">
@@ -4939,10 +4948,10 @@
         <v>311</v>
       </c>
       <c r="B310" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C310" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.4">
@@ -4950,10 +4959,10 @@
         <v>312</v>
       </c>
       <c r="B311" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C311" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.4">
@@ -4961,10 +4970,10 @@
         <v>313</v>
       </c>
       <c r="B312" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C312" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.4">
@@ -4972,10 +4981,10 @@
         <v>314</v>
       </c>
       <c r="B313" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C313" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.4">
@@ -4983,10 +4992,10 @@
         <v>315</v>
       </c>
       <c r="B314" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C314" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.4">
@@ -4994,10 +5003,10 @@
         <v>316</v>
       </c>
       <c r="B315" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C315" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.4">
@@ -5005,10 +5014,10 @@
         <v>317</v>
       </c>
       <c r="B316" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C316" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.4">
@@ -5016,10 +5025,10 @@
         <v>318</v>
       </c>
       <c r="B317" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C317" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.4">
@@ -5027,10 +5036,10 @@
         <v>319</v>
       </c>
       <c r="B318" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C318" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.4">
@@ -5038,10 +5047,10 @@
         <v>320</v>
       </c>
       <c r="B319" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C319" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.4">
@@ -5049,10 +5058,10 @@
         <v>321</v>
       </c>
       <c r="B320" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C320" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.4">
@@ -5060,10 +5069,10 @@
         <v>322</v>
       </c>
       <c r="B321" s="1">
-        <v>0.34329999999999994</v>
+        <v>0.33258999999999994</v>
       </c>
       <c r="C321" s="1">
-        <v>0.78160000000000007</v>
+        <v>0.77698</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generate data upto 2022/01/31 (나중에 revert할 것임)
</commit_message>
<xml_diff>
--- a/data/vaccine/vaccine_efficacy.xlsx
+++ b/data/vaccine/vaccine_efficacy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dropbox (Jeongjoo)\estimation_matlab\Covid19_seoul_gyeonggi\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yjlee/repos/COVID19_SeoulGyeonggi/data/vaccine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95679DDC-0841-4072-ACF5-8693DC9F1487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9109FA29-57B1-D741-9587-BF70E728E927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="776" yWindow="3181" windowWidth="15765" windowHeight="12772" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="3180" windowWidth="15760" windowHeight="12780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="354">
   <si>
     <t>date/vaccine efficacy
 (AZ+PFIZER, average)</t>
@@ -1002,13 +1002,106 @@
   </si>
   <si>
     <t>2021.12.31</t>
+  </si>
+  <si>
+    <t>2022.01.01</t>
+  </si>
+  <si>
+    <t>2022.01.02</t>
+  </si>
+  <si>
+    <t>2022.01.03</t>
+  </si>
+  <si>
+    <t>2022.01.04</t>
+  </si>
+  <si>
+    <t>2022.01.05</t>
+  </si>
+  <si>
+    <t>2022.01.06</t>
+  </si>
+  <si>
+    <t>2022.01.07</t>
+  </si>
+  <si>
+    <t>2022.01.08</t>
+  </si>
+  <si>
+    <t>2022.01.09</t>
+  </si>
+  <si>
+    <t>2022.01.10</t>
+  </si>
+  <si>
+    <t>2022.01.11</t>
+  </si>
+  <si>
+    <t>2022.01.12</t>
+  </si>
+  <si>
+    <t>2022.01.13</t>
+  </si>
+  <si>
+    <t>2022.01.14</t>
+  </si>
+  <si>
+    <t>2022.01.15</t>
+  </si>
+  <si>
+    <t>2022.01.16</t>
+  </si>
+  <si>
+    <t>2022.01.17</t>
+  </si>
+  <si>
+    <t>2022.01.18</t>
+  </si>
+  <si>
+    <t>2022.01.19</t>
+  </si>
+  <si>
+    <t>2022.01.20</t>
+  </si>
+  <si>
+    <t>2022.01.21</t>
+  </si>
+  <si>
+    <t>2022.01.22</t>
+  </si>
+  <si>
+    <t>2022.01.23</t>
+  </si>
+  <si>
+    <t>2022.01.24</t>
+  </si>
+  <si>
+    <t>2022.01.25</t>
+  </si>
+  <si>
+    <t>2022.01.26</t>
+  </si>
+  <si>
+    <t>2022.01.27</t>
+  </si>
+  <si>
+    <t>2022.01.28</t>
+  </si>
+  <si>
+    <t>2022.01.29</t>
+  </si>
+  <si>
+    <t>2022.01.30</t>
+  </si>
+  <si>
+    <t>2022.01.31</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1065,7 +1158,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
     <dxf>
@@ -1532,19 +1625,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C321"/>
+  <dimension ref="A1:C352"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A333" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="F344" sqref="F344"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="18.2" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="18.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="32.6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="32.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1555,7 +1648,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>218</v>
       </c>
@@ -1566,7 +1659,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>222</v>
       </c>
@@ -1577,7 +1670,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>221</v>
       </c>
@@ -1588,7 +1681,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>223</v>
       </c>
@@ -1599,7 +1692,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>219</v>
       </c>
@@ -1610,7 +1703,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>220</v>
       </c>
@@ -1621,7 +1714,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>228</v>
       </c>
@@ -1632,7 +1725,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>227</v>
       </c>
@@ -1643,7 +1736,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
         <v>224</v>
       </c>
@@ -1654,7 +1747,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
         <v>226</v>
       </c>
@@ -1665,7 +1758,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
         <v>225</v>
       </c>
@@ -1676,7 +1769,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
         <v>229</v>
       </c>
@@ -1687,7 +1780,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
         <v>230</v>
       </c>
@@ -1698,7 +1791,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
         <v>217</v>
       </c>
@@ -1709,7 +1802,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1720,7 +1813,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -1731,7 +1824,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
         <v>140</v>
       </c>
@@ -1742,7 +1835,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
         <v>149</v>
       </c>
@@ -1753,7 +1846,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
         <v>152</v>
       </c>
@@ -1764,7 +1857,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
         <v>15</v>
       </c>
@@ -1775,7 +1868,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
         <v>141</v>
       </c>
@@ -1786,7 +1879,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
         <v>144</v>
       </c>
@@ -1797,7 +1890,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -1808,7 +1901,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
         <v>42</v>
       </c>
@@ -1819,7 +1912,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
@@ -1830,7 +1923,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
         <v>147</v>
       </c>
@@ -1841,7 +1934,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -1852,7 +1945,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
         <v>22</v>
       </c>
@@ -1863,7 +1956,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
         <v>34</v>
       </c>
@@ -1874,7 +1967,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
         <v>150</v>
       </c>
@@ -1885,7 +1978,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
         <v>143</v>
       </c>
@@ -1896,7 +1989,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
         <v>154</v>
       </c>
@@ -1907,7 +2000,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
         <v>16</v>
       </c>
@@ -1918,7 +2011,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
         <v>31</v>
       </c>
@@ -1929,7 +2022,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
         <v>145</v>
       </c>
@@ -1940,7 +2033,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
         <v>29</v>
       </c>
@@ -1951,7 +2044,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:3">
       <c r="A38" s="1" t="s">
         <v>17</v>
       </c>
@@ -1962,7 +2055,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:3">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -1973,7 +2066,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:3">
       <c r="A40" s="1" t="s">
         <v>25</v>
       </c>
@@ -1984,7 +2077,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
         <v>53</v>
       </c>
@@ -1995,7 +2088,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:3">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
@@ -2006,7 +2099,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:3">
       <c r="A43" s="1" t="s">
         <v>19</v>
       </c>
@@ -2017,7 +2110,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:3">
       <c r="A44" s="1" t="s">
         <v>37</v>
       </c>
@@ -2028,7 +2121,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
         <v>41</v>
       </c>
@@ -2039,7 +2132,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:3">
       <c r="A46" s="1" t="s">
         <v>32</v>
       </c>
@@ -2050,7 +2143,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:3">
       <c r="A47" s="1" t="s">
         <v>58</v>
       </c>
@@ -2061,7 +2154,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:3">
       <c r="A48" s="1" t="s">
         <v>56</v>
       </c>
@@ -2072,7 +2165,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
         <v>23</v>
       </c>
@@ -2083,7 +2176,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:3">
       <c r="A50" s="1" t="s">
         <v>36</v>
       </c>
@@ -2094,7 +2187,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:3">
       <c r="A51" s="1" t="s">
         <v>24</v>
       </c>
@@ -2105,7 +2198,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:3">
       <c r="A52" s="1" t="s">
         <v>130</v>
       </c>
@@ -2116,7 +2209,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
         <v>139</v>
       </c>
@@ -2127,7 +2220,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:3">
       <c r="A54" s="1" t="s">
         <v>128</v>
       </c>
@@ -2138,7 +2231,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:3">
       <c r="A55" s="1" t="s">
         <v>153</v>
       </c>
@@ -2149,7 +2242,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:3">
       <c r="A56" s="1" t="s">
         <v>30</v>
       </c>
@@ -2160,7 +2253,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:3">
       <c r="A57" s="1" t="s">
         <v>28</v>
       </c>
@@ -2171,7 +2264,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:3">
       <c r="A58" s="1" t="s">
         <v>146</v>
       </c>
@@ -2182,7 +2275,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:3">
       <c r="A59" s="1" t="s">
         <v>126</v>
       </c>
@@ -2193,7 +2286,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:3">
       <c r="A60" s="1" t="s">
         <v>142</v>
       </c>
@@ -2204,7 +2297,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:3">
       <c r="A61" s="1" t="s">
         <v>151</v>
       </c>
@@ -2215,7 +2308,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:3">
       <c r="A62" s="1" t="s">
         <v>127</v>
       </c>
@@ -2226,7 +2319,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:3">
       <c r="A63" s="1" t="s">
         <v>134</v>
       </c>
@@ -2237,7 +2330,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:3">
       <c r="A64" s="1" t="s">
         <v>136</v>
       </c>
@@ -2248,7 +2341,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:3">
       <c r="A65" s="1" t="s">
         <v>148</v>
       </c>
@@ -2259,7 +2352,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:3">
       <c r="A66" s="1" t="s">
         <v>124</v>
       </c>
@@ -2270,7 +2363,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:3">
       <c r="A67" s="1" t="s">
         <v>135</v>
       </c>
@@ -2281,7 +2374,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:3">
       <c r="A68" s="1" t="s">
         <v>125</v>
       </c>
@@ -2292,7 +2385,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:3">
       <c r="A69" s="1" t="s">
         <v>138</v>
       </c>
@@ -2303,7 +2396,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:3">
       <c r="A70" s="1" t="s">
         <v>129</v>
       </c>
@@ -2314,7 +2407,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:3">
       <c r="A71" s="1" t="s">
         <v>74</v>
       </c>
@@ -2325,7 +2418,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:3">
       <c r="A72" s="1" t="s">
         <v>78</v>
       </c>
@@ -2336,7 +2429,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:3">
       <c r="A73" s="1" t="s">
         <v>63</v>
       </c>
@@ -2347,7 +2440,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:3">
       <c r="A74" s="1" t="s">
         <v>70</v>
       </c>
@@ -2358,7 +2451,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:3">
       <c r="A75" s="1" t="s">
         <v>69</v>
       </c>
@@ -2369,7 +2462,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:3">
       <c r="A76" s="1" t="s">
         <v>67</v>
       </c>
@@ -2380,7 +2473,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:3">
       <c r="A77" s="1" t="s">
         <v>66</v>
       </c>
@@ -2391,7 +2484,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:3">
       <c r="A78" s="1" t="s">
         <v>72</v>
       </c>
@@ -2402,7 +2495,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:3">
       <c r="A79" s="1" t="s">
         <v>73</v>
       </c>
@@ -2413,7 +2506,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:3">
       <c r="A80" s="1" t="s">
         <v>64</v>
       </c>
@@ -2424,7 +2517,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:3">
       <c r="A81" s="1" t="s">
         <v>75</v>
       </c>
@@ -2435,7 +2528,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:3">
       <c r="A82" s="1" t="s">
         <v>162</v>
       </c>
@@ -2446,7 +2539,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:3">
       <c r="A83" s="1" t="s">
         <v>80</v>
       </c>
@@ -2457,7 +2550,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:3">
       <c r="A84" s="1" t="s">
         <v>87</v>
       </c>
@@ -2468,7 +2561,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:3">
       <c r="A85" s="1" t="s">
         <v>79</v>
       </c>
@@ -2479,7 +2572,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:3">
       <c r="A86" s="1" t="s">
         <v>86</v>
       </c>
@@ -2490,7 +2583,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:3">
       <c r="A87" s="1" t="s">
         <v>85</v>
       </c>
@@ -2501,7 +2594,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:3">
       <c r="A88" s="1" t="s">
         <v>170</v>
       </c>
@@ -2512,7 +2605,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:3">
       <c r="A89" s="1" t="s">
         <v>91</v>
       </c>
@@ -2523,7 +2616,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:3">
       <c r="A90" s="1" t="s">
         <v>77</v>
       </c>
@@ -2534,7 +2627,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:3">
       <c r="A91" s="1" t="s">
         <v>88</v>
       </c>
@@ -2545,7 +2638,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:3">
       <c r="A92" s="1" t="s">
         <v>81</v>
       </c>
@@ -2556,7 +2649,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:3">
       <c r="A93" s="1" t="s">
         <v>90</v>
       </c>
@@ -2567,7 +2660,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:3">
       <c r="A94" s="1" t="s">
         <v>84</v>
       </c>
@@ -2578,7 +2671,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:3">
       <c r="A95" s="1" t="s">
         <v>166</v>
       </c>
@@ -2589,7 +2682,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:3">
       <c r="A96" s="1" t="s">
         <v>83</v>
       </c>
@@ -2600,7 +2693,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:3">
       <c r="A97" s="1" t="s">
         <v>89</v>
       </c>
@@ -2611,7 +2704,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:3">
       <c r="A98" s="1" t="s">
         <v>168</v>
       </c>
@@ -2622,7 +2715,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:3">
       <c r="A99" s="1" t="s">
         <v>173</v>
       </c>
@@ -2633,7 +2726,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:3">
       <c r="A100" s="1" t="s">
         <v>155</v>
       </c>
@@ -2644,7 +2737,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:3">
       <c r="A101" s="1" t="s">
         <v>167</v>
       </c>
@@ -2655,7 +2748,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:3">
       <c r="A102" s="1" t="s">
         <v>177</v>
       </c>
@@ -2666,7 +2759,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:3">
       <c r="A103" s="1" t="s">
         <v>160</v>
       </c>
@@ -2677,7 +2770,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:3">
       <c r="A104" s="1" t="s">
         <v>179</v>
       </c>
@@ -2688,7 +2781,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:3">
       <c r="A105" s="1" t="s">
         <v>163</v>
       </c>
@@ -2699,7 +2792,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:3">
       <c r="A106" s="1" t="s">
         <v>169</v>
       </c>
@@ -2710,7 +2803,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:3">
       <c r="A107" s="1" t="s">
         <v>156</v>
       </c>
@@ -2721,7 +2814,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:3">
       <c r="A108" s="1" t="s">
         <v>164</v>
       </c>
@@ -2732,7 +2825,7 @@
         <v>0.83941599999999994</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:3">
       <c r="A109" s="1" t="s">
         <v>165</v>
       </c>
@@ -2743,7 +2836,7 @@
         <v>0.83941599999999994</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:3">
       <c r="A110" s="1" t="s">
         <v>159</v>
       </c>
@@ -2754,7 +2847,7 @@
         <v>0.83941599999999994</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:3">
       <c r="A111" s="1" t="s">
         <v>157</v>
       </c>
@@ -2765,7 +2858,7 @@
         <v>0.83941599999999994</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:3">
       <c r="A112" s="1" t="s">
         <v>161</v>
       </c>
@@ -2776,7 +2869,7 @@
         <v>0.83941599999999994</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:3">
       <c r="A113" s="1" t="s">
         <v>158</v>
       </c>
@@ -2787,7 +2880,7 @@
         <v>0.83959456559766765</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:3">
       <c r="A114" s="1" t="s">
         <v>95</v>
       </c>
@@ -2798,7 +2891,7 @@
         <v>0.83974407580174915</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:3">
       <c r="A115" s="1" t="s">
         <v>180</v>
       </c>
@@ -2809,7 +2902,7 @@
         <v>0.83986510787172008</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:3">
       <c r="A116" s="1" t="s">
         <v>93</v>
       </c>
@@ -2820,7 +2913,7 @@
         <v>0.83995823906705536</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:3">
       <c r="A117" s="1" t="s">
         <v>178</v>
       </c>
@@ -2831,7 +2924,7 @@
         <v>0.84002404664723029</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:3">
       <c r="A118" s="1" t="s">
         <v>182</v>
       </c>
@@ -2842,7 +2935,7 @@
         <v>0.84006310787172012</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:3">
       <c r="A119" s="1" t="s">
         <v>172</v>
       </c>
@@ -2853,7 +2946,7 @@
         <v>0.84007599999999993</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:3">
       <c r="A120" s="1" t="s">
         <v>183</v>
       </c>
@@ -2864,7 +2957,7 @@
         <v>0.84004647874789007</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:3">
       <c r="A121" s="1" t="s">
         <v>171</v>
       </c>
@@ -2875,7 +2968,7 @@
         <v>0.83996771827528005</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:3">
       <c r="A122" s="1" t="s">
         <v>176</v>
       </c>
@@ -2886,7 +2979,7 @@
         <v>0.83985442350774886</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:3">
       <c r="A123" s="1" t="s">
         <v>174</v>
       </c>
@@ -2897,7 +2990,7 @@
         <v>0.83972129937087614</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:3">
       <c r="A124" s="1" t="s">
         <v>184</v>
       </c>
@@ -2908,7 +3001,7 @@
         <v>0.83958305079024098</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:3">
       <c r="A125" s="1" t="s">
         <v>96</v>
       </c>
@@ -2919,7 +3012,7 @@
         <v>0.83945438269142236</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:3">
       <c r="A126" s="1" t="s">
         <v>181</v>
       </c>
@@ -2930,7 +3023,7 @@
         <v>0.83934999999999993</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:3">
       <c r="A127" s="1" t="s">
         <v>185</v>
       </c>
@@ -2941,7 +3034,7 @@
         <v>0.83927306053606165</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:3">
       <c r="A128" s="1" t="s">
         <v>92</v>
       </c>
@@ -2952,7 +3045,7 @@
         <v>0.83921112051225688</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:3">
       <c r="A129" s="1" t="s">
         <v>175</v>
       </c>
@@ -2963,7 +3056,7 @@
         <v>0.83915548244300764</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:3">
       <c r="A130" s="1" t="s">
         <v>106</v>
       </c>
@@ -2974,7 +3067,7 @@
         <v>0.83909744884273563</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:3">
       <c r="A131" s="1" t="s">
         <v>99</v>
       </c>
@@ -2985,7 +3078,7 @@
         <v>0.83902832222586243</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:3">
       <c r="A132" s="1" t="s">
         <v>104</v>
       </c>
@@ -2996,7 +3089,7 @@
         <v>0.83893940510681009</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:3">
       <c r="A133" s="1" t="s">
         <v>102</v>
       </c>
@@ -3007,7 +3100,7 @@
         <v>0.83882199999999996</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:3">
       <c r="A134" s="1" t="s">
         <v>107</v>
       </c>
@@ -3018,7 +3111,7 @@
         <v>0.83858395941060593</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:3">
       <c r="A135" s="1" t="s">
         <v>103</v>
       </c>
@@ -3029,7 +3122,7 @@
         <v>0.83816147786620443</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:3">
       <c r="A136" s="1" t="s">
         <v>98</v>
       </c>
@@ -3040,7 +3133,7 @@
         <v>0.83758837091482152</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:3">
       <c r="A137" s="1" t="s">
         <v>120</v>
       </c>
@@ -3051,7 +3144,7 @@
         <v>0.83689845410448349</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:3">
       <c r="A138" s="1" t="s">
         <v>94</v>
       </c>
@@ -3062,7 +3155,7 @@
         <v>0.8361255429832164</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:3">
       <c r="A139" s="1" t="s">
         <v>115</v>
       </c>
@@ -3073,7 +3166,7 @@
         <v>0.83530345309904652</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:3">
       <c r="A140" s="1" t="s">
         <v>118</v>
       </c>
@@ -3084,7 +3177,7 @@
         <v>0.83446600000000004</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:3">
       <c r="A141" s="1" t="s">
         <v>101</v>
       </c>
@@ -3095,7 +3188,7 @@
         <v>0.83350012174927124</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:3">
       <c r="A142" s="1" t="s">
         <v>100</v>
       </c>
@@ -3106,7 +3199,7 @@
         <v>0.83231731195335279</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:3">
       <c r="A143" s="1" t="s">
         <v>119</v>
       </c>
@@ -3117,7 +3210,7 @@
         <v>0.8309882194752185</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:3">
       <c r="A144" s="1" t="s">
         <v>105</v>
       </c>
@@ -3128,7 +3221,7 @@
         <v>0.82958349317784252</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:3">
       <c r="A145" s="1" t="s">
         <v>97</v>
       </c>
@@ -3139,7 +3232,7 @@
         <v>0.82817378192419822</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:3">
       <c r="A146" s="1" t="s">
         <v>114</v>
       </c>
@@ -3150,7 +3243,7 @@
         <v>0.8268297345772595</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:3">
       <c r="A147" s="1" t="s">
         <v>137</v>
       </c>
@@ -3161,7 +3254,7 @@
         <v>0.82562200000000008</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:3">
       <c r="A148" s="1" t="s">
         <v>122</v>
       </c>
@@ -3172,7 +3265,7 @@
         <v>0.82455424727753457</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:3">
       <c r="A149" s="1" t="s">
         <v>123</v>
       </c>
@@ -3183,7 +3276,7 @@
         <v>0.82356196711559126</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:3">
       <c r="A150" s="1" t="s">
         <v>133</v>
       </c>
@@ -3194,7 +3287,7 @@
         <v>0.82261354080806404</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:3">
       <c r="A151" s="1" t="s">
         <v>113</v>
       </c>
@@ -3205,7 +3298,7 @@
         <v>0.82167734964884731</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:3">
       <c r="A152" s="1" t="s">
         <v>108</v>
       </c>
@@ -3216,7 +3309,7 @@
         <v>0.82072177493183507</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:3">
       <c r="A153" s="1" t="s">
         <v>111</v>
       </c>
@@ -3227,7 +3320,7 @@
         <v>0.81971519795092129</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:3">
       <c r="A154" s="1" t="s">
         <v>121</v>
       </c>
@@ -3238,7 +3331,7 @@
         <v>0.81862599999999996</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:3">
       <c r="A155" s="1" t="s">
         <v>110</v>
       </c>
@@ -3249,7 +3342,7 @@
         <v>0.8174314346260847</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:3">
       <c r="A156" s="1" t="s">
         <v>112</v>
       </c>
@@ -3260,7 +3353,7 @@
         <v>0.81614757175342278</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:3">
       <c r="A157" s="1" t="s">
         <v>116</v>
       </c>
@@ -3271,7 +3364,7 @@
         <v>0.8148010172417598</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="158" spans="1:3">
       <c r="A158" s="1" t="s">
         <v>117</v>
       </c>
@@ -3282,7 +3375,7 @@
         <v>0.81341837695084074</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:3">
       <c r="A159" s="1" t="s">
         <v>109</v>
       </c>
@@ -3293,7 +3386,7 @@
         <v>0.81202625674041085</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:3">
       <c r="A160" s="1" t="s">
         <v>132</v>
       </c>
@@ -3304,7 +3397,7 @@
         <v>0.81065126247021557</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:3">
       <c r="A161" s="1" t="s">
         <v>131</v>
       </c>
@@ -3315,7 +3408,7 @@
         <v>0.80932000000000004</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="162" spans="1:3">
       <c r="A162" s="1" t="s">
         <v>206</v>
       </c>
@@ -3326,7 +3419,7 @@
         <v>0.80801501511257534</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="163" spans="1:3">
       <c r="A163" s="1" t="s">
         <v>65</v>
       </c>
@@ -3337,7 +3430,7 @@
         <v>0.8067067229573277</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="164" spans="1:3">
       <c r="A164" s="1" t="s">
         <v>207</v>
       </c>
@@ -3348,7 +3441,7 @@
         <v>0.80540353344386428</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:3">
       <c r="A165" s="1" t="s">
         <v>71</v>
       </c>
@@ -3359,7 +3452,7 @@
         <v>0.80411385648179245</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:3">
       <c r="A166" s="1" t="s">
         <v>82</v>
       </c>
@@ -3370,7 +3463,7 @@
         <v>0.8028461019807196</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:3">
       <c r="A167" s="1" t="s">
         <v>215</v>
       </c>
@@ -3381,7 +3474,7 @@
         <v>0.80160867985025286</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:3">
       <c r="A168" s="1" t="s">
         <v>76</v>
       </c>
@@ -3392,7 +3485,7 @@
         <v>0.80041000000000007</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:3">
       <c r="A169" s="1" t="s">
         <v>68</v>
       </c>
@@ -3403,7 +3496,7 @@
         <v>0.79925883582469492</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="170" spans="1:3">
       <c r="A170" s="1" t="s">
         <v>192</v>
       </c>
@@ -3414,7 +3507,7 @@
         <v>0.7981493448269299</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="171" spans="1:3">
       <c r="A171" s="1" t="s">
         <v>210</v>
       </c>
@@ -3425,7 +3518,7 @@
         <v>0.79706801307809894</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="172" spans="1:3">
       <c r="A172" s="1" t="s">
         <v>193</v>
       </c>
@@ -3436,7 +3529,7 @@
         <v>0.79600132664959633</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:3">
       <c r="A173" s="1" t="s">
         <v>198</v>
       </c>
@@ -3447,7 +3540,7 @@
         <v>0.79493577161281626</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="174" spans="1:3">
       <c r="A174" s="1" t="s">
         <v>199</v>
       </c>
@@ -3458,7 +3551,7 @@
         <v>0.79385783403915267</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="175" spans="1:3">
       <c r="A175" s="1" t="s">
         <v>216</v>
       </c>
@@ -3469,7 +3562,7 @@
         <v>0.79275400000000007</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="176" spans="1:3">
       <c r="A176" s="1" t="s">
         <v>200</v>
       </c>
@@ -3480,7 +3573,7 @@
         <v>0.79155758162530321</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="177" spans="1:3">
       <c r="A177" s="1" t="s">
         <v>190</v>
       </c>
@@ -3491,7 +3584,7 @@
         <v>0.79025822618026798</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="178" spans="1:3">
       <c r="A178" s="1" t="s">
         <v>61</v>
       </c>
@@ -3502,7 +3595,7 @@
         <v>0.78892692243917972</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="179" spans="1:3">
       <c r="A179" s="1" t="s">
         <v>186</v>
       </c>
@@ -3513,7 +3606,7 @@
         <v>0.78763465917632358</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="180" spans="1:3">
       <c r="A180" s="1" t="s">
         <v>195</v>
       </c>
@@ -3524,7 +3617,7 @@
         <v>0.78645242516598479</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="181" spans="1:3">
       <c r="A181" s="1" t="s">
         <v>62</v>
       </c>
@@ -3535,7 +3628,7 @@
         <v>0.7854512091824486</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="182" spans="1:3">
       <c r="A182" s="1" t="s">
         <v>204</v>
       </c>
@@ -3546,7 +3639,7 @@
         <v>0.78470200000000001</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="183" spans="1:3">
       <c r="A183" s="1" t="s">
         <v>209</v>
       </c>
@@ -3557,7 +3650,7 @@
         <v>0.78415616326530613</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="184" spans="1:3">
       <c r="A184" s="1" t="s">
         <v>197</v>
       </c>
@@ -3568,7 +3661,7 @@
         <v>0.78370042176870758</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="185" spans="1:3">
       <c r="A185" s="1" t="s">
         <v>213</v>
       </c>
@@ -3579,7 +3672,7 @@
         <v>0.78330880000000003</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="186" spans="1:3">
       <c r="A186" s="1" t="s">
         <v>202</v>
       </c>
@@ -3590,7 +3683,7 @@
         <v>0.78295532244897958</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="187" spans="1:3">
       <c r="A187" s="1" t="s">
         <v>208</v>
       </c>
@@ -3601,7 +3694,7 @@
         <v>0.78261401360544225</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="188" spans="1:3">
       <c r="A188" s="1" t="s">
         <v>212</v>
       </c>
@@ -3612,7 +3705,7 @@
         <v>0.78225889795918369</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="189" spans="1:3">
       <c r="A189" s="1" t="s">
         <v>211</v>
       </c>
@@ -3623,7 +3716,7 @@
         <v>0.781864</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="190" spans="1:3">
       <c r="A190" s="1" t="s">
         <v>214</v>
       </c>
@@ -3634,7 +3727,7 @@
         <v>0.78142066160271062</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="191" spans="1:3">
       <c r="A191" s="1" t="s">
         <v>205</v>
       </c>
@@ -3645,7 +3738,7 @@
         <v>0.78094892643080405</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="192" spans="1:3">
       <c r="A192" s="1" t="s">
         <v>43</v>
       </c>
@@ -3656,7 +3749,7 @@
         <v>0.78046587165707992</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="193" spans="1:3">
       <c r="A193" s="1" t="s">
         <v>35</v>
       </c>
@@ -3667,7 +3760,7 @@
         <v>0.77998857445433767</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="194" spans="1:3">
       <c r="A194" s="1" t="s">
         <v>44</v>
       </c>
@@ -3678,7 +3771,7 @@
         <v>0.77953411199537725</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="195" spans="1:3">
       <c r="A195" s="1" t="s">
         <v>39</v>
       </c>
@@ -3689,7 +3782,7 @@
         <v>0.77911956145299821</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="196" spans="1:3">
       <c r="A196" s="1" t="s">
         <v>45</v>
       </c>
@@ -3700,7 +3793,7 @@
         <v>0.77876199999999995</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="197" spans="1:3">
       <c r="A197" s="1" t="s">
         <v>46</v>
       </c>
@@ -3711,7 +3804,7 @@
         <v>0.778445334173824</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="198" spans="1:3">
       <c r="A198" s="1" t="s">
         <v>51</v>
       </c>
@@ -3722,7 +3815,7 @@
         <v>0.77814416594437008</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="199" spans="1:3">
       <c r="A199" s="1" t="s">
         <v>50</v>
       </c>
@@ -3733,7 +3826,7 @@
         <v>0.77786161563312584</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="200" spans="1:3">
       <c r="A200" s="1" t="s">
         <v>4</v>
       </c>
@@ -3744,7 +3837,7 @@
         <v>0.77760080356157901</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="201" spans="1:3">
       <c r="A201" s="1" t="s">
         <v>201</v>
       </c>
@@ -3755,7 +3848,7 @@
         <v>0.77736485005121747</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="202" spans="1:3">
       <c r="A202" s="1" t="s">
         <v>189</v>
       </c>
@@ -3766,7 +3859,7 @@
         <v>0.77715687542352851</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="203" spans="1:3">
       <c r="A203" s="1" t="s">
         <v>194</v>
       </c>
@@ -3777,7 +3870,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="204" spans="1:3">
       <c r="A204" s="1" t="s">
         <v>14</v>
       </c>
@@ -3788,7 +3881,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="205" spans="1:3">
       <c r="A205" s="1" t="s">
         <v>8</v>
       </c>
@@ -3799,7 +3892,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="206" spans="1:3">
       <c r="A206" s="1" t="s">
         <v>7</v>
       </c>
@@ -3810,7 +3903,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="207" spans="1:3">
       <c r="A207" s="1" t="s">
         <v>12</v>
       </c>
@@ -3821,7 +3914,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="208" spans="1:3">
       <c r="A208" s="1" t="s">
         <v>13</v>
       </c>
@@ -3832,7 +3925,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="209" spans="1:3">
       <c r="A209" s="1" t="s">
         <v>188</v>
       </c>
@@ -3843,7 +3936,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="210" spans="1:3">
       <c r="A210" s="1" t="s">
         <v>196</v>
       </c>
@@ -3854,7 +3947,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="211" spans="1:3">
       <c r="A211" s="1" t="s">
         <v>2</v>
       </c>
@@ -3865,7 +3958,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="212" spans="1:3">
       <c r="A212" s="1" t="s">
         <v>191</v>
       </c>
@@ -3876,7 +3969,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="213" spans="1:3">
       <c r="A213" s="1" t="s">
         <v>187</v>
       </c>
@@ -3887,7 +3980,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="214" spans="1:3">
       <c r="A214" s="1" t="s">
         <v>1</v>
       </c>
@@ -3898,7 +3991,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="215" spans="1:3">
       <c r="A215" s="1" t="s">
         <v>3</v>
       </c>
@@ -3909,7 +4002,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="216" spans="1:3">
       <c r="A216" s="1" t="s">
         <v>55</v>
       </c>
@@ -3920,7 +4013,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="217" spans="1:3">
       <c r="A217" s="1" t="s">
         <v>57</v>
       </c>
@@ -3931,7 +4024,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="218" spans="1:3">
       <c r="A218" s="1" t="s">
         <v>11</v>
       </c>
@@ -3942,7 +4035,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="219" spans="1:3">
       <c r="A219" s="1" t="s">
         <v>9</v>
       </c>
@@ -3953,7 +4046,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="220" spans="1:3">
       <c r="A220" s="1" t="s">
         <v>47</v>
       </c>
@@ -3964,7 +4057,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="221" spans="1:3">
       <c r="A221" s="1" t="s">
         <v>60</v>
       </c>
@@ -3975,7 +4068,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="222" spans="1:3">
       <c r="A222" s="1" t="s">
         <v>10</v>
       </c>
@@ -3986,7 +4079,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="223" spans="1:3">
       <c r="A223" s="1" t="s">
         <v>52</v>
       </c>
@@ -3997,7 +4090,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="224" spans="1:3">
       <c r="A224" s="1" t="s">
         <v>59</v>
       </c>
@@ -4008,7 +4101,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="225" spans="1:3">
       <c r="A225" s="1" t="s">
         <v>49</v>
       </c>
@@ -4019,7 +4112,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="226" spans="1:3">
       <c r="A226" s="1" t="s">
         <v>48</v>
       </c>
@@ -4030,7 +4123,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="227" spans="1:3">
       <c r="A227" s="1" t="s">
         <v>5</v>
       </c>
@@ -4041,7 +4134,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="228" spans="1:3">
       <c r="A228" s="1" t="s">
         <v>6</v>
       </c>
@@ -4052,7 +4145,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="229" spans="1:3">
       <c r="A229" s="1" t="s">
         <v>203</v>
       </c>
@@ -4063,7 +4156,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="230" spans="1:3">
       <c r="A230" s="3" t="s">
         <v>231</v>
       </c>
@@ -4074,7 +4167,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="231" spans="1:3">
       <c r="A231" s="3" t="s">
         <v>232</v>
       </c>
@@ -4085,7 +4178,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="232" spans="1:3">
       <c r="A232" s="3" t="s">
         <v>233</v>
       </c>
@@ -4096,7 +4189,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="233" spans="1:3">
       <c r="A233" s="3" t="s">
         <v>234</v>
       </c>
@@ -4107,7 +4200,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="234" spans="1:3">
       <c r="A234" s="3" t="s">
         <v>235</v>
       </c>
@@ -4118,7 +4211,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="235" spans="1:3">
       <c r="A235" s="3" t="s">
         <v>236</v>
       </c>
@@ -4129,7 +4222,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="236" spans="1:3">
       <c r="A236" s="3" t="s">
         <v>237</v>
       </c>
@@ -4140,7 +4233,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="237" spans="1:3">
       <c r="A237" s="3" t="s">
         <v>238</v>
       </c>
@@ -4151,7 +4244,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="238" spans="1:3">
       <c r="A238" s="3" t="s">
         <v>239</v>
       </c>
@@ -4162,7 +4255,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="239" spans="1:3">
       <c r="A239" s="3" t="s">
         <v>240</v>
       </c>
@@ -4173,7 +4266,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="240" spans="1:3">
       <c r="A240" s="3" t="s">
         <v>241</v>
       </c>
@@ -4184,7 +4277,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="241" spans="1:3">
       <c r="A241" s="3" t="s">
         <v>242</v>
       </c>
@@ -4195,7 +4288,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="242" spans="1:3">
       <c r="A242" s="3" t="s">
         <v>243</v>
       </c>
@@ -4206,7 +4299,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="243" spans="1:3">
       <c r="A243" s="3" t="s">
         <v>244</v>
       </c>
@@ -4217,7 +4310,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="244" spans="1:3">
       <c r="A244" s="3" t="s">
         <v>245</v>
       </c>
@@ -4228,7 +4321,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="245" spans="1:3">
       <c r="A245" s="3" t="s">
         <v>246</v>
       </c>
@@ -4239,7 +4332,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="246" spans="1:3">
       <c r="A246" s="3" t="s">
         <v>247</v>
       </c>
@@ -4250,7 +4343,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="247" spans="1:3">
       <c r="A247" s="3" t="s">
         <v>248</v>
       </c>
@@ -4261,7 +4354,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="248" spans="1:3">
       <c r="A248" s="3" t="s">
         <v>249</v>
       </c>
@@ -4272,7 +4365,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="249" spans="1:3">
       <c r="A249" s="3" t="s">
         <v>250</v>
       </c>
@@ -4283,7 +4376,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="250" spans="1:3">
       <c r="A250" s="3" t="s">
         <v>251</v>
       </c>
@@ -4294,7 +4387,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="251" spans="1:3">
       <c r="A251" s="3" t="s">
         <v>252</v>
       </c>
@@ -4305,7 +4398,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="252" spans="1:3">
       <c r="A252" s="3" t="s">
         <v>253</v>
       </c>
@@ -4316,7 +4409,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="253" spans="1:3">
       <c r="A253" s="3" t="s">
         <v>254</v>
       </c>
@@ -4327,7 +4420,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="254" spans="1:3">
       <c r="A254" s="3" t="s">
         <v>255</v>
       </c>
@@ -4338,7 +4431,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="255" spans="1:3">
       <c r="A255" s="3" t="s">
         <v>256</v>
       </c>
@@ -4349,7 +4442,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="256" spans="1:3">
       <c r="A256" s="3" t="s">
         <v>257</v>
       </c>
@@ -4360,7 +4453,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="257" spans="1:3">
       <c r="A257" s="3" t="s">
         <v>258</v>
       </c>
@@ -4371,7 +4464,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="258" spans="1:3">
       <c r="A258" s="3" t="s">
         <v>259</v>
       </c>
@@ -4382,7 +4475,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="259" spans="1:3">
       <c r="A259" s="3" t="s">
         <v>260</v>
       </c>
@@ -4393,7 +4486,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="260" spans="1:3">
       <c r="A260" s="3" t="s">
         <v>261</v>
       </c>
@@ -4404,7 +4497,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="261" spans="1:3">
       <c r="A261" s="3" t="s">
         <v>262</v>
       </c>
@@ -4415,7 +4508,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="262" spans="1:3">
       <c r="A262" s="3" t="s">
         <v>263</v>
       </c>
@@ -4426,7 +4519,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="263" spans="1:3">
       <c r="A263" s="3" t="s">
         <v>264</v>
       </c>
@@ -4437,7 +4530,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="264" spans="1:3">
       <c r="A264" s="3" t="s">
         <v>265</v>
       </c>
@@ -4448,7 +4541,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="265" spans="1:3">
       <c r="A265" s="3" t="s">
         <v>266</v>
       </c>
@@ -4459,7 +4552,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="266" spans="1:3">
       <c r="A266" s="3" t="s">
         <v>267</v>
       </c>
@@ -4470,7 +4563,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="267" spans="1:3">
       <c r="A267" s="3" t="s">
         <v>268</v>
       </c>
@@ -4481,7 +4574,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="268" spans="1:3">
       <c r="A268" s="3" t="s">
         <v>269</v>
       </c>
@@ -4492,7 +4585,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="269" spans="1:3">
       <c r="A269" s="3" t="s">
         <v>270</v>
       </c>
@@ -4503,7 +4596,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="270" spans="1:3">
       <c r="A270" s="3" t="s">
         <v>271</v>
       </c>
@@ -4514,7 +4607,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="271" spans="1:3">
       <c r="A271" s="3" t="s">
         <v>272</v>
       </c>
@@ -4525,7 +4618,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="272" spans="1:3">
       <c r="A272" s="3" t="s">
         <v>273</v>
       </c>
@@ -4536,7 +4629,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="273" spans="1:3">
       <c r="A273" s="3" t="s">
         <v>274</v>
       </c>
@@ -4547,7 +4640,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="274" spans="1:3">
       <c r="A274" s="3" t="s">
         <v>275</v>
       </c>
@@ -4558,7 +4651,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="275" spans="1:3">
       <c r="A275" s="3" t="s">
         <v>276</v>
       </c>
@@ -4569,7 +4662,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="276" spans="1:3">
       <c r="A276" s="3" t="s">
         <v>277</v>
       </c>
@@ -4580,7 +4673,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="277" spans="1:3">
       <c r="A277" s="3" t="s">
         <v>278</v>
       </c>
@@ -4591,7 +4684,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="278" spans="1:3">
       <c r="A278" s="3" t="s">
         <v>279</v>
       </c>
@@ -4602,7 +4695,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="279" spans="1:3">
       <c r="A279" s="3" t="s">
         <v>280</v>
       </c>
@@ -4613,7 +4706,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="280" spans="1:3">
       <c r="A280" s="3" t="s">
         <v>281</v>
       </c>
@@ -4624,7 +4717,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="281" spans="1:3">
       <c r="A281" s="3" t="s">
         <v>282</v>
       </c>
@@ -4635,7 +4728,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="282" spans="1:3">
       <c r="A282" s="3" t="s">
         <v>283</v>
       </c>
@@ -4646,7 +4739,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="283" spans="1:3">
       <c r="A283" s="3" t="s">
         <v>284</v>
       </c>
@@ -4657,7 +4750,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="284" spans="1:3">
       <c r="A284" s="3" t="s">
         <v>285</v>
       </c>
@@ -4668,7 +4761,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="285" spans="1:3">
       <c r="A285" s="3" t="s">
         <v>286</v>
       </c>
@@ -4679,7 +4772,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="286" spans="1:3">
       <c r="A286" s="3" t="s">
         <v>287</v>
       </c>
@@ -4690,7 +4783,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="287" spans="1:3">
       <c r="A287" s="3" t="s">
         <v>288</v>
       </c>
@@ -4701,7 +4794,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="288" spans="1:3">
       <c r="A288" s="3" t="s">
         <v>289</v>
       </c>
@@ -4712,7 +4805,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="289" spans="1:3">
       <c r="A289" s="3" t="s">
         <v>290</v>
       </c>
@@ -4723,7 +4816,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="290" spans="1:3">
       <c r="A290" s="3" t="s">
         <v>291</v>
       </c>
@@ -4734,7 +4827,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="291" spans="1:3">
       <c r="A291" s="3" t="s">
         <v>292</v>
       </c>
@@ -4745,7 +4838,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="292" spans="1:3">
       <c r="A292" s="3" t="s">
         <v>293</v>
       </c>
@@ -4756,7 +4849,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="293" spans="1:3">
       <c r="A293" s="3" t="s">
         <v>294</v>
       </c>
@@ -4767,7 +4860,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="294" spans="1:3">
       <c r="A294" s="3" t="s">
         <v>295</v>
       </c>
@@ -4778,7 +4871,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="295" spans="1:3">
       <c r="A295" s="3" t="s">
         <v>296</v>
       </c>
@@ -4789,7 +4882,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="296" spans="1:3">
       <c r="A296" s="3" t="s">
         <v>297</v>
       </c>
@@ -4800,7 +4893,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="297" spans="1:3">
       <c r="A297" s="3" t="s">
         <v>298</v>
       </c>
@@ -4811,7 +4904,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="298" spans="1:3">
       <c r="A298" s="3" t="s">
         <v>299</v>
       </c>
@@ -4822,7 +4915,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="299" spans="1:3">
       <c r="A299" s="3" t="s">
         <v>300</v>
       </c>
@@ -4833,7 +4926,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="300" spans="1:3">
       <c r="A300" s="3" t="s">
         <v>301</v>
       </c>
@@ -4844,7 +4937,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="301" spans="1:3">
       <c r="A301" s="3" t="s">
         <v>302</v>
       </c>
@@ -4855,7 +4948,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="302" spans="1:3">
       <c r="A302" s="3" t="s">
         <v>303</v>
       </c>
@@ -4866,7 +4959,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="303" spans="1:3">
       <c r="A303" s="3" t="s">
         <v>304</v>
       </c>
@@ -4877,7 +4970,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="304" spans="1:3">
       <c r="A304" s="3" t="s">
         <v>305</v>
       </c>
@@ -4888,7 +4981,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="305" spans="1:3">
       <c r="A305" s="3" t="s">
         <v>306</v>
       </c>
@@ -4899,7 +4992,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="306" spans="1:3">
       <c r="A306" s="3" t="s">
         <v>307</v>
       </c>
@@ -4910,7 +5003,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="307" spans="1:3">
       <c r="A307" s="3" t="s">
         <v>308</v>
       </c>
@@ -4921,7 +5014,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="308" spans="1:3">
       <c r="A308" s="3" t="s">
         <v>309</v>
       </c>
@@ -4932,7 +5025,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="309" spans="1:3">
       <c r="A309" s="3" t="s">
         <v>310</v>
       </c>
@@ -4943,7 +5036,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="310" spans="1:3">
       <c r="A310" s="3" t="s">
         <v>311</v>
       </c>
@@ -4954,7 +5047,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="311" spans="1:3">
       <c r="A311" s="3" t="s">
         <v>312</v>
       </c>
@@ -4965,7 +5058,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="312" spans="1:3">
       <c r="A312" s="3" t="s">
         <v>313</v>
       </c>
@@ -4976,7 +5069,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="313" spans="1:3">
       <c r="A313" s="3" t="s">
         <v>314</v>
       </c>
@@ -4987,7 +5080,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="314" spans="1:3">
       <c r="A314" s="3" t="s">
         <v>315</v>
       </c>
@@ -4998,7 +5091,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="315" spans="1:3">
       <c r="A315" s="3" t="s">
         <v>316</v>
       </c>
@@ -5009,7 +5102,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="316" spans="1:3">
       <c r="A316" s="3" t="s">
         <v>317</v>
       </c>
@@ -5020,7 +5113,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="317" spans="1:3">
       <c r="A317" s="3" t="s">
         <v>318</v>
       </c>
@@ -5031,7 +5124,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="318" spans="1:3">
       <c r="A318" s="3" t="s">
         <v>319</v>
       </c>
@@ -5042,7 +5135,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="319" spans="1:3">
       <c r="A319" s="3" t="s">
         <v>320</v>
       </c>
@@ -5053,7 +5146,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="320" spans="1:3">
       <c r="A320" s="3" t="s">
         <v>321</v>
       </c>
@@ -5064,7 +5157,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="321" spans="1:3">
       <c r="A321" s="3" t="s">
         <v>322</v>
       </c>
@@ -5072,6 +5165,347 @@
         <v>0.33258999999999994</v>
       </c>
       <c r="C321" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3">
+      <c r="A322" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="B322" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C322" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3">
+      <c r="A323" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="B323" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C323" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3">
+      <c r="A324" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="B324" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C324" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3">
+      <c r="A325" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="B325" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C325" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3">
+      <c r="A326" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="B326" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C326" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3">
+      <c r="A327" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="B327" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C327" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3">
+      <c r="A328" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B328" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C328" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3">
+      <c r="A329" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="B329" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C329" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3">
+      <c r="A330" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="B330" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C330" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3">
+      <c r="A331" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B331" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C331" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3">
+      <c r="A332" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="B332" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C332" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3">
+      <c r="A333" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="B333" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C333" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3">
+      <c r="A334" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B334" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C334" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3">
+      <c r="A335" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="B335" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C335" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3">
+      <c r="A336" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="B336" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C336" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3">
+      <c r="A337" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="B337" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C337" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3">
+      <c r="A338" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B338" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C338" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3">
+      <c r="A339" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="B339" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C339" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3">
+      <c r="A340" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="B340" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C340" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3">
+      <c r="A341" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="B341" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C341" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3">
+      <c r="A342" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="B342" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C342" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3">
+      <c r="A343" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="B343" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C343" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3">
+      <c r="A344" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="B344" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C344" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="345" spans="1:3">
+      <c r="A345" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B345" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C345" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3">
+      <c r="A346" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B346" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C346" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3">
+      <c r="A347" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="B347" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C347" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="348" spans="1:3">
+      <c r="A348" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="B348" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C348" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="349" spans="1:3">
+      <c r="A349" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="B349" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C349" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="350" spans="1:3">
+      <c r="A350" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="B350" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C350" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="351" spans="1:3">
+      <c r="A351" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="B351" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C351" s="1">
+        <v>0.77698</v>
+      </c>
+    </row>
+    <row r="352" spans="1:3">
+      <c r="A352" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="B352" s="1">
+        <v>0.33258999999999994</v>
+      </c>
+      <c r="C352" s="1">
         <v>0.77698</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "generate data upto 2022/01/31 (나중에 revert할 것임)"
This reverts commit 9e08393f22ad001b94e682471600cc78ae6b4edc.
</commit_message>
<xml_diff>
--- a/data/vaccine/vaccine_efficacy.xlsx
+++ b/data/vaccine/vaccine_efficacy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yjlee/repos/COVID19_SeoulGyeonggi/data/vaccine/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dropbox (Jeongjoo)\estimation_matlab\Covid19_seoul_gyeonggi\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9109FA29-57B1-D741-9587-BF70E728E927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95679DDC-0841-4072-ACF5-8693DC9F1487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="3180" windowWidth="15760" windowHeight="12780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="776" yWindow="3181" windowWidth="15765" windowHeight="12772" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="323">
   <si>
     <t>date/vaccine efficacy
 (AZ+PFIZER, average)</t>
@@ -1002,106 +1002,13 @@
   </si>
   <si>
     <t>2021.12.31</t>
-  </si>
-  <si>
-    <t>2022.01.01</t>
-  </si>
-  <si>
-    <t>2022.01.02</t>
-  </si>
-  <si>
-    <t>2022.01.03</t>
-  </si>
-  <si>
-    <t>2022.01.04</t>
-  </si>
-  <si>
-    <t>2022.01.05</t>
-  </si>
-  <si>
-    <t>2022.01.06</t>
-  </si>
-  <si>
-    <t>2022.01.07</t>
-  </si>
-  <si>
-    <t>2022.01.08</t>
-  </si>
-  <si>
-    <t>2022.01.09</t>
-  </si>
-  <si>
-    <t>2022.01.10</t>
-  </si>
-  <si>
-    <t>2022.01.11</t>
-  </si>
-  <si>
-    <t>2022.01.12</t>
-  </si>
-  <si>
-    <t>2022.01.13</t>
-  </si>
-  <si>
-    <t>2022.01.14</t>
-  </si>
-  <si>
-    <t>2022.01.15</t>
-  </si>
-  <si>
-    <t>2022.01.16</t>
-  </si>
-  <si>
-    <t>2022.01.17</t>
-  </si>
-  <si>
-    <t>2022.01.18</t>
-  </si>
-  <si>
-    <t>2022.01.19</t>
-  </si>
-  <si>
-    <t>2022.01.20</t>
-  </si>
-  <si>
-    <t>2022.01.21</t>
-  </si>
-  <si>
-    <t>2022.01.22</t>
-  </si>
-  <si>
-    <t>2022.01.23</t>
-  </si>
-  <si>
-    <t>2022.01.24</t>
-  </si>
-  <si>
-    <t>2022.01.25</t>
-  </si>
-  <si>
-    <t>2022.01.26</t>
-  </si>
-  <si>
-    <t>2022.01.27</t>
-  </si>
-  <si>
-    <t>2022.01.28</t>
-  </si>
-  <si>
-    <t>2022.01.29</t>
-  </si>
-  <si>
-    <t>2022.01.30</t>
-  </si>
-  <si>
-    <t>2022.01.31</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1158,7 +1065,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
     <dxf>
@@ -1625,19 +1532,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C352"/>
+  <dimension ref="A1:C321"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A333" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="F344" sqref="F344"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="18.2" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.69921875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="32.5" customHeight="1">
+    <row r="1" spans="1:3" ht="32.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1648,7 +1555,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>218</v>
       </c>
@@ -1659,7 +1566,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>222</v>
       </c>
@@ -1670,7 +1577,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>221</v>
       </c>
@@ -1681,7 +1588,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>223</v>
       </c>
@@ -1692,7 +1599,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>219</v>
       </c>
@@ -1703,7 +1610,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>220</v>
       </c>
@@ -1714,7 +1621,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>228</v>
       </c>
@@ -1725,7 +1632,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>227</v>
       </c>
@@ -1736,7 +1643,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>224</v>
       </c>
@@ -1747,7 +1654,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>226</v>
       </c>
@@ -1758,7 +1665,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>225</v>
       </c>
@@ -1769,7 +1676,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>229</v>
       </c>
@@ -1780,7 +1687,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>230</v>
       </c>
@@ -1791,7 +1698,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>217</v>
       </c>
@@ -1802,7 +1709,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1813,7 +1720,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -1824,7 +1731,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>140</v>
       </c>
@@ -1835,7 +1742,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>149</v>
       </c>
@@ -1846,7 +1753,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>152</v>
       </c>
@@ -1857,7 +1764,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>15</v>
       </c>
@@ -1868,7 +1775,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>141</v>
       </c>
@@ -1879,7 +1786,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>144</v>
       </c>
@@ -1890,7 +1797,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -1901,7 +1808,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>42</v>
       </c>
@@ -1912,7 +1819,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
@@ -1923,7 +1830,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>147</v>
       </c>
@@ -1934,7 +1841,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -1945,7 +1852,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
         <v>22</v>
       </c>
@@ -1956,7 +1863,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
         <v>34</v>
       </c>
@@ -1967,7 +1874,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
         <v>150</v>
       </c>
@@ -1978,7 +1885,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
         <v>143</v>
       </c>
@@ -1989,7 +1896,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
         <v>154</v>
       </c>
@@ -2000,7 +1907,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
         <v>16</v>
       </c>
@@ -2011,7 +1918,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
         <v>31</v>
       </c>
@@ -2022,7 +1929,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
         <v>145</v>
       </c>
@@ -2033,7 +1940,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
         <v>29</v>
       </c>
@@ -2044,7 +1951,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
         <v>17</v>
       </c>
@@ -2055,7 +1962,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -2066,7 +1973,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
         <v>25</v>
       </c>
@@ -2077,7 +1984,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
         <v>53</v>
       </c>
@@ -2088,7 +1995,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
@@ -2099,7 +2006,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A43" s="1" t="s">
         <v>19</v>
       </c>
@@ -2110,7 +2017,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
         <v>37</v>
       </c>
@@ -2121,7 +2028,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A45" s="1" t="s">
         <v>41</v>
       </c>
@@ -2132,7 +2039,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A46" s="1" t="s">
         <v>32</v>
       </c>
@@ -2143,7 +2050,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A47" s="1" t="s">
         <v>58</v>
       </c>
@@ -2154,7 +2061,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A48" s="1" t="s">
         <v>56</v>
       </c>
@@ -2165,7 +2072,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A49" s="1" t="s">
         <v>23</v>
       </c>
@@ -2176,7 +2083,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A50" s="1" t="s">
         <v>36</v>
       </c>
@@ -2187,7 +2094,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A51" s="1" t="s">
         <v>24</v>
       </c>
@@ -2198,7 +2105,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A52" s="1" t="s">
         <v>130</v>
       </c>
@@ -2209,7 +2116,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A53" s="1" t="s">
         <v>139</v>
       </c>
@@ -2220,7 +2127,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A54" s="1" t="s">
         <v>128</v>
       </c>
@@ -2231,7 +2138,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A55" s="1" t="s">
         <v>153</v>
       </c>
@@ -2242,7 +2149,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A56" s="1" t="s">
         <v>30</v>
       </c>
@@ -2253,7 +2160,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A57" s="1" t="s">
         <v>28</v>
       </c>
@@ -2264,7 +2171,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A58" s="1" t="s">
         <v>146</v>
       </c>
@@ -2275,7 +2182,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A59" s="1" t="s">
         <v>126</v>
       </c>
@@ -2286,7 +2193,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A60" s="1" t="s">
         <v>142</v>
       </c>
@@ -2297,7 +2204,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A61" s="1" t="s">
         <v>151</v>
       </c>
@@ -2308,7 +2215,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A62" s="1" t="s">
         <v>127</v>
       </c>
@@ -2319,7 +2226,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A63" s="1" t="s">
         <v>134</v>
       </c>
@@ -2330,7 +2237,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A64" s="1" t="s">
         <v>136</v>
       </c>
@@ -2341,7 +2248,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A65" s="1" t="s">
         <v>148</v>
       </c>
@@ -2352,7 +2259,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A66" s="1" t="s">
         <v>124</v>
       </c>
@@ -2363,7 +2270,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A67" s="1" t="s">
         <v>135</v>
       </c>
@@ -2374,7 +2281,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A68" s="1" t="s">
         <v>125</v>
       </c>
@@ -2385,7 +2292,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A69" s="1" t="s">
         <v>138</v>
       </c>
@@ -2396,7 +2303,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A70" s="1" t="s">
         <v>129</v>
       </c>
@@ -2407,7 +2314,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A71" s="1" t="s">
         <v>74</v>
       </c>
@@ -2418,7 +2325,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A72" s="1" t="s">
         <v>78</v>
       </c>
@@ -2429,7 +2336,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A73" s="1" t="s">
         <v>63</v>
       </c>
@@ -2440,7 +2347,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A74" s="1" t="s">
         <v>70</v>
       </c>
@@ -2451,7 +2358,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A75" s="1" t="s">
         <v>69</v>
       </c>
@@ -2462,7 +2369,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A76" s="1" t="s">
         <v>67</v>
       </c>
@@ -2473,7 +2380,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A77" s="1" t="s">
         <v>66</v>
       </c>
@@ -2484,7 +2391,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A78" s="1" t="s">
         <v>72</v>
       </c>
@@ -2495,7 +2402,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A79" s="1" t="s">
         <v>73</v>
       </c>
@@ -2506,7 +2413,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A80" s="1" t="s">
         <v>64</v>
       </c>
@@ -2517,7 +2424,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A81" s="1" t="s">
         <v>75</v>
       </c>
@@ -2528,7 +2435,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A82" s="1" t="s">
         <v>162</v>
       </c>
@@ -2539,7 +2446,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A83" s="1" t="s">
         <v>80</v>
       </c>
@@ -2550,7 +2457,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A84" s="1" t="s">
         <v>87</v>
       </c>
@@ -2561,7 +2468,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A85" s="1" t="s">
         <v>79</v>
       </c>
@@ -2572,7 +2479,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A86" s="1" t="s">
         <v>86</v>
       </c>
@@ -2583,7 +2490,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A87" s="1" t="s">
         <v>85</v>
       </c>
@@ -2594,7 +2501,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A88" s="1" t="s">
         <v>170</v>
       </c>
@@ -2605,7 +2512,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A89" s="1" t="s">
         <v>91</v>
       </c>
@@ -2616,7 +2523,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A90" s="1" t="s">
         <v>77</v>
       </c>
@@ -2627,7 +2534,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A91" s="1" t="s">
         <v>88</v>
       </c>
@@ -2638,7 +2545,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A92" s="1" t="s">
         <v>81</v>
       </c>
@@ -2649,7 +2556,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A93" s="1" t="s">
         <v>90</v>
       </c>
@@ -2660,7 +2567,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A94" s="1" t="s">
         <v>84</v>
       </c>
@@ -2671,7 +2578,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A95" s="1" t="s">
         <v>166</v>
       </c>
@@ -2682,7 +2589,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A96" s="1" t="s">
         <v>83</v>
       </c>
@@ -2693,7 +2600,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A97" s="1" t="s">
         <v>89</v>
       </c>
@@ -2704,7 +2611,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A98" s="1" t="s">
         <v>168</v>
       </c>
@@ -2715,7 +2622,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A99" s="1" t="s">
         <v>173</v>
       </c>
@@ -2726,7 +2633,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A100" s="1" t="s">
         <v>155</v>
       </c>
@@ -2737,7 +2644,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A101" s="1" t="s">
         <v>167</v>
       </c>
@@ -2748,7 +2655,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A102" s="1" t="s">
         <v>177</v>
       </c>
@@ -2759,7 +2666,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A103" s="1" t="s">
         <v>160</v>
       </c>
@@ -2770,7 +2677,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A104" s="1" t="s">
         <v>179</v>
       </c>
@@ -2781,7 +2688,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A105" s="1" t="s">
         <v>163</v>
       </c>
@@ -2792,7 +2699,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A106" s="1" t="s">
         <v>169</v>
       </c>
@@ -2803,7 +2710,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A107" s="1" t="s">
         <v>156</v>
       </c>
@@ -2814,7 +2721,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A108" s="1" t="s">
         <v>164</v>
       </c>
@@ -2825,7 +2732,7 @@
         <v>0.83941599999999994</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A109" s="1" t="s">
         <v>165</v>
       </c>
@@ -2836,7 +2743,7 @@
         <v>0.83941599999999994</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A110" s="1" t="s">
         <v>159</v>
       </c>
@@ -2847,7 +2754,7 @@
         <v>0.83941599999999994</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A111" s="1" t="s">
         <v>157</v>
       </c>
@@ -2858,7 +2765,7 @@
         <v>0.83941599999999994</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A112" s="1" t="s">
         <v>161</v>
       </c>
@@ -2869,7 +2776,7 @@
         <v>0.83941599999999994</v>
       </c>
     </row>
-    <row r="113" spans="1:3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A113" s="1" t="s">
         <v>158</v>
       </c>
@@ -2880,7 +2787,7 @@
         <v>0.83959456559766765</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A114" s="1" t="s">
         <v>95</v>
       </c>
@@ -2891,7 +2798,7 @@
         <v>0.83974407580174915</v>
       </c>
     </row>
-    <row r="115" spans="1:3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A115" s="1" t="s">
         <v>180</v>
       </c>
@@ -2902,7 +2809,7 @@
         <v>0.83986510787172008</v>
       </c>
     </row>
-    <row r="116" spans="1:3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A116" s="1" t="s">
         <v>93</v>
       </c>
@@ -2913,7 +2820,7 @@
         <v>0.83995823906705536</v>
       </c>
     </row>
-    <row r="117" spans="1:3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A117" s="1" t="s">
         <v>178</v>
       </c>
@@ -2924,7 +2831,7 @@
         <v>0.84002404664723029</v>
       </c>
     </row>
-    <row r="118" spans="1:3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A118" s="1" t="s">
         <v>182</v>
       </c>
@@ -2935,7 +2842,7 @@
         <v>0.84006310787172012</v>
       </c>
     </row>
-    <row r="119" spans="1:3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A119" s="1" t="s">
         <v>172</v>
       </c>
@@ -2946,7 +2853,7 @@
         <v>0.84007599999999993</v>
       </c>
     </row>
-    <row r="120" spans="1:3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A120" s="1" t="s">
         <v>183</v>
       </c>
@@ -2957,7 +2864,7 @@
         <v>0.84004647874789007</v>
       </c>
     </row>
-    <row r="121" spans="1:3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A121" s="1" t="s">
         <v>171</v>
       </c>
@@ -2968,7 +2875,7 @@
         <v>0.83996771827528005</v>
       </c>
     </row>
-    <row r="122" spans="1:3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A122" s="1" t="s">
         <v>176</v>
       </c>
@@ -2979,7 +2886,7 @@
         <v>0.83985442350774886</v>
       </c>
     </row>
-    <row r="123" spans="1:3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A123" s="1" t="s">
         <v>174</v>
       </c>
@@ -2990,7 +2897,7 @@
         <v>0.83972129937087614</v>
       </c>
     </row>
-    <row r="124" spans="1:3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A124" s="1" t="s">
         <v>184</v>
       </c>
@@ -3001,7 +2908,7 @@
         <v>0.83958305079024098</v>
       </c>
     </row>
-    <row r="125" spans="1:3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A125" s="1" t="s">
         <v>96</v>
       </c>
@@ -3012,7 +2919,7 @@
         <v>0.83945438269142236</v>
       </c>
     </row>
-    <row r="126" spans="1:3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A126" s="1" t="s">
         <v>181</v>
       </c>
@@ -3023,7 +2930,7 @@
         <v>0.83934999999999993</v>
       </c>
     </row>
-    <row r="127" spans="1:3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A127" s="1" t="s">
         <v>185</v>
       </c>
@@ -3034,7 +2941,7 @@
         <v>0.83927306053606165</v>
       </c>
     </row>
-    <row r="128" spans="1:3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A128" s="1" t="s">
         <v>92</v>
       </c>
@@ -3045,7 +2952,7 @@
         <v>0.83921112051225688</v>
       </c>
     </row>
-    <row r="129" spans="1:3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A129" s="1" t="s">
         <v>175</v>
       </c>
@@ -3056,7 +2963,7 @@
         <v>0.83915548244300764</v>
       </c>
     </row>
-    <row r="130" spans="1:3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A130" s="1" t="s">
         <v>106</v>
       </c>
@@ -3067,7 +2974,7 @@
         <v>0.83909744884273563</v>
       </c>
     </row>
-    <row r="131" spans="1:3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A131" s="1" t="s">
         <v>99</v>
       </c>
@@ -3078,7 +2985,7 @@
         <v>0.83902832222586243</v>
       </c>
     </row>
-    <row r="132" spans="1:3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A132" s="1" t="s">
         <v>104</v>
       </c>
@@ -3089,7 +2996,7 @@
         <v>0.83893940510681009</v>
       </c>
     </row>
-    <row r="133" spans="1:3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A133" s="1" t="s">
         <v>102</v>
       </c>
@@ -3100,7 +3007,7 @@
         <v>0.83882199999999996</v>
       </c>
     </row>
-    <row r="134" spans="1:3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A134" s="1" t="s">
         <v>107</v>
       </c>
@@ -3111,7 +3018,7 @@
         <v>0.83858395941060593</v>
       </c>
     </row>
-    <row r="135" spans="1:3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A135" s="1" t="s">
         <v>103</v>
       </c>
@@ -3122,7 +3029,7 @@
         <v>0.83816147786620443</v>
       </c>
     </row>
-    <row r="136" spans="1:3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A136" s="1" t="s">
         <v>98</v>
       </c>
@@ -3133,7 +3040,7 @@
         <v>0.83758837091482152</v>
       </c>
     </row>
-    <row r="137" spans="1:3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A137" s="1" t="s">
         <v>120</v>
       </c>
@@ -3144,7 +3051,7 @@
         <v>0.83689845410448349</v>
       </c>
     </row>
-    <row r="138" spans="1:3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A138" s="1" t="s">
         <v>94</v>
       </c>
@@ -3155,7 +3062,7 @@
         <v>0.8361255429832164</v>
       </c>
     </row>
-    <row r="139" spans="1:3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A139" s="1" t="s">
         <v>115</v>
       </c>
@@ -3166,7 +3073,7 @@
         <v>0.83530345309904652</v>
       </c>
     </row>
-    <row r="140" spans="1:3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A140" s="1" t="s">
         <v>118</v>
       </c>
@@ -3177,7 +3084,7 @@
         <v>0.83446600000000004</v>
       </c>
     </row>
-    <row r="141" spans="1:3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A141" s="1" t="s">
         <v>101</v>
       </c>
@@ -3188,7 +3095,7 @@
         <v>0.83350012174927124</v>
       </c>
     </row>
-    <row r="142" spans="1:3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A142" s="1" t="s">
         <v>100</v>
       </c>
@@ -3199,7 +3106,7 @@
         <v>0.83231731195335279</v>
       </c>
     </row>
-    <row r="143" spans="1:3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A143" s="1" t="s">
         <v>119</v>
       </c>
@@ -3210,7 +3117,7 @@
         <v>0.8309882194752185</v>
       </c>
     </row>
-    <row r="144" spans="1:3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A144" s="1" t="s">
         <v>105</v>
       </c>
@@ -3221,7 +3128,7 @@
         <v>0.82958349317784252</v>
       </c>
     </row>
-    <row r="145" spans="1:3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A145" s="1" t="s">
         <v>97</v>
       </c>
@@ -3232,7 +3139,7 @@
         <v>0.82817378192419822</v>
       </c>
     </row>
-    <row r="146" spans="1:3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A146" s="1" t="s">
         <v>114</v>
       </c>
@@ -3243,7 +3150,7 @@
         <v>0.8268297345772595</v>
       </c>
     </row>
-    <row r="147" spans="1:3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A147" s="1" t="s">
         <v>137</v>
       </c>
@@ -3254,7 +3161,7 @@
         <v>0.82562200000000008</v>
       </c>
     </row>
-    <row r="148" spans="1:3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A148" s="1" t="s">
         <v>122</v>
       </c>
@@ -3265,7 +3172,7 @@
         <v>0.82455424727753457</v>
       </c>
     </row>
-    <row r="149" spans="1:3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A149" s="1" t="s">
         <v>123</v>
       </c>
@@ -3276,7 +3183,7 @@
         <v>0.82356196711559126</v>
       </c>
     </row>
-    <row r="150" spans="1:3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A150" s="1" t="s">
         <v>133</v>
       </c>
@@ -3287,7 +3194,7 @@
         <v>0.82261354080806404</v>
       </c>
     </row>
-    <row r="151" spans="1:3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A151" s="1" t="s">
         <v>113</v>
       </c>
@@ -3298,7 +3205,7 @@
         <v>0.82167734964884731</v>
       </c>
     </row>
-    <row r="152" spans="1:3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A152" s="1" t="s">
         <v>108</v>
       </c>
@@ -3309,7 +3216,7 @@
         <v>0.82072177493183507</v>
       </c>
     </row>
-    <row r="153" spans="1:3">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A153" s="1" t="s">
         <v>111</v>
       </c>
@@ -3320,7 +3227,7 @@
         <v>0.81971519795092129</v>
       </c>
     </row>
-    <row r="154" spans="1:3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A154" s="1" t="s">
         <v>121</v>
       </c>
@@ -3331,7 +3238,7 @@
         <v>0.81862599999999996</v>
       </c>
     </row>
-    <row r="155" spans="1:3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A155" s="1" t="s">
         <v>110</v>
       </c>
@@ -3342,7 +3249,7 @@
         <v>0.8174314346260847</v>
       </c>
     </row>
-    <row r="156" spans="1:3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A156" s="1" t="s">
         <v>112</v>
       </c>
@@ -3353,7 +3260,7 @@
         <v>0.81614757175342278</v>
       </c>
     </row>
-    <row r="157" spans="1:3">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A157" s="1" t="s">
         <v>116</v>
       </c>
@@ -3364,7 +3271,7 @@
         <v>0.8148010172417598</v>
       </c>
     </row>
-    <row r="158" spans="1:3">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A158" s="1" t="s">
         <v>117</v>
       </c>
@@ -3375,7 +3282,7 @@
         <v>0.81341837695084074</v>
       </c>
     </row>
-    <row r="159" spans="1:3">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A159" s="1" t="s">
         <v>109</v>
       </c>
@@ -3386,7 +3293,7 @@
         <v>0.81202625674041085</v>
       </c>
     </row>
-    <row r="160" spans="1:3">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A160" s="1" t="s">
         <v>132</v>
       </c>
@@ -3397,7 +3304,7 @@
         <v>0.81065126247021557</v>
       </c>
     </row>
-    <row r="161" spans="1:3">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A161" s="1" t="s">
         <v>131</v>
       </c>
@@ -3408,7 +3315,7 @@
         <v>0.80932000000000004</v>
       </c>
     </row>
-    <row r="162" spans="1:3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A162" s="1" t="s">
         <v>206</v>
       </c>
@@ -3419,7 +3326,7 @@
         <v>0.80801501511257534</v>
       </c>
     </row>
-    <row r="163" spans="1:3">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A163" s="1" t="s">
         <v>65</v>
       </c>
@@ -3430,7 +3337,7 @@
         <v>0.8067067229573277</v>
       </c>
     </row>
-    <row r="164" spans="1:3">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A164" s="1" t="s">
         <v>207</v>
       </c>
@@ -3441,7 +3348,7 @@
         <v>0.80540353344386428</v>
       </c>
     </row>
-    <row r="165" spans="1:3">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A165" s="1" t="s">
         <v>71</v>
       </c>
@@ -3452,7 +3359,7 @@
         <v>0.80411385648179245</v>
       </c>
     </row>
-    <row r="166" spans="1:3">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A166" s="1" t="s">
         <v>82</v>
       </c>
@@ -3463,7 +3370,7 @@
         <v>0.8028461019807196</v>
       </c>
     </row>
-    <row r="167" spans="1:3">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A167" s="1" t="s">
         <v>215</v>
       </c>
@@ -3474,7 +3381,7 @@
         <v>0.80160867985025286</v>
       </c>
     </row>
-    <row r="168" spans="1:3">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A168" s="1" t="s">
         <v>76</v>
       </c>
@@ -3485,7 +3392,7 @@
         <v>0.80041000000000007</v>
       </c>
     </row>
-    <row r="169" spans="1:3">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A169" s="1" t="s">
         <v>68</v>
       </c>
@@ -3496,7 +3403,7 @@
         <v>0.79925883582469492</v>
       </c>
     </row>
-    <row r="170" spans="1:3">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A170" s="1" t="s">
         <v>192</v>
       </c>
@@ -3507,7 +3414,7 @@
         <v>0.7981493448269299</v>
       </c>
     </row>
-    <row r="171" spans="1:3">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A171" s="1" t="s">
         <v>210</v>
       </c>
@@ -3518,7 +3425,7 @@
         <v>0.79706801307809894</v>
       </c>
     </row>
-    <row r="172" spans="1:3">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A172" s="1" t="s">
         <v>193</v>
       </c>
@@ -3529,7 +3436,7 @@
         <v>0.79600132664959633</v>
       </c>
     </row>
-    <row r="173" spans="1:3">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A173" s="1" t="s">
         <v>198</v>
       </c>
@@ -3540,7 +3447,7 @@
         <v>0.79493577161281626</v>
       </c>
     </row>
-    <row r="174" spans="1:3">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A174" s="1" t="s">
         <v>199</v>
       </c>
@@ -3551,7 +3458,7 @@
         <v>0.79385783403915267</v>
       </c>
     </row>
-    <row r="175" spans="1:3">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A175" s="1" t="s">
         <v>216</v>
       </c>
@@ -3562,7 +3469,7 @@
         <v>0.79275400000000007</v>
       </c>
     </row>
-    <row r="176" spans="1:3">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A176" s="1" t="s">
         <v>200</v>
       </c>
@@ -3573,7 +3480,7 @@
         <v>0.79155758162530321</v>
       </c>
     </row>
-    <row r="177" spans="1:3">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A177" s="1" t="s">
         <v>190</v>
       </c>
@@ -3584,7 +3491,7 @@
         <v>0.79025822618026798</v>
       </c>
     </row>
-    <row r="178" spans="1:3">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A178" s="1" t="s">
         <v>61</v>
       </c>
@@ -3595,7 +3502,7 @@
         <v>0.78892692243917972</v>
       </c>
     </row>
-    <row r="179" spans="1:3">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A179" s="1" t="s">
         <v>186</v>
       </c>
@@ -3606,7 +3513,7 @@
         <v>0.78763465917632358</v>
       </c>
     </row>
-    <row r="180" spans="1:3">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A180" s="1" t="s">
         <v>195</v>
       </c>
@@ -3617,7 +3524,7 @@
         <v>0.78645242516598479</v>
       </c>
     </row>
-    <row r="181" spans="1:3">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A181" s="1" t="s">
         <v>62</v>
       </c>
@@ -3628,7 +3535,7 @@
         <v>0.7854512091824486</v>
       </c>
     </row>
-    <row r="182" spans="1:3">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A182" s="1" t="s">
         <v>204</v>
       </c>
@@ -3639,7 +3546,7 @@
         <v>0.78470200000000001</v>
       </c>
     </row>
-    <row r="183" spans="1:3">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A183" s="1" t="s">
         <v>209</v>
       </c>
@@ -3650,7 +3557,7 @@
         <v>0.78415616326530613</v>
       </c>
     </row>
-    <row r="184" spans="1:3">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A184" s="1" t="s">
         <v>197</v>
       </c>
@@ -3661,7 +3568,7 @@
         <v>0.78370042176870758</v>
       </c>
     </row>
-    <row r="185" spans="1:3">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A185" s="1" t="s">
         <v>213</v>
       </c>
@@ -3672,7 +3579,7 @@
         <v>0.78330880000000003</v>
       </c>
     </row>
-    <row r="186" spans="1:3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A186" s="1" t="s">
         <v>202</v>
       </c>
@@ -3683,7 +3590,7 @@
         <v>0.78295532244897958</v>
       </c>
     </row>
-    <row r="187" spans="1:3">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A187" s="1" t="s">
         <v>208</v>
       </c>
@@ -3694,7 +3601,7 @@
         <v>0.78261401360544225</v>
       </c>
     </row>
-    <row r="188" spans="1:3">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A188" s="1" t="s">
         <v>212</v>
       </c>
@@ -3705,7 +3612,7 @@
         <v>0.78225889795918369</v>
       </c>
     </row>
-    <row r="189" spans="1:3">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A189" s="1" t="s">
         <v>211</v>
       </c>
@@ -3716,7 +3623,7 @@
         <v>0.781864</v>
       </c>
     </row>
-    <row r="190" spans="1:3">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A190" s="1" t="s">
         <v>214</v>
       </c>
@@ -3727,7 +3634,7 @@
         <v>0.78142066160271062</v>
       </c>
     </row>
-    <row r="191" spans="1:3">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A191" s="1" t="s">
         <v>205</v>
       </c>
@@ -3738,7 +3645,7 @@
         <v>0.78094892643080405</v>
       </c>
     </row>
-    <row r="192" spans="1:3">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A192" s="1" t="s">
         <v>43</v>
       </c>
@@ -3749,7 +3656,7 @@
         <v>0.78046587165707992</v>
       </c>
     </row>
-    <row r="193" spans="1:3">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A193" s="1" t="s">
         <v>35</v>
       </c>
@@ -3760,7 +3667,7 @@
         <v>0.77998857445433767</v>
       </c>
     </row>
-    <row r="194" spans="1:3">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A194" s="1" t="s">
         <v>44</v>
       </c>
@@ -3771,7 +3678,7 @@
         <v>0.77953411199537725</v>
       </c>
     </row>
-    <row r="195" spans="1:3">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A195" s="1" t="s">
         <v>39</v>
       </c>
@@ -3782,7 +3689,7 @@
         <v>0.77911956145299821</v>
       </c>
     </row>
-    <row r="196" spans="1:3">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A196" s="1" t="s">
         <v>45</v>
       </c>
@@ -3793,7 +3700,7 @@
         <v>0.77876199999999995</v>
       </c>
     </row>
-    <row r="197" spans="1:3">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A197" s="1" t="s">
         <v>46</v>
       </c>
@@ -3804,7 +3711,7 @@
         <v>0.778445334173824</v>
       </c>
     </row>
-    <row r="198" spans="1:3">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A198" s="1" t="s">
         <v>51</v>
       </c>
@@ -3815,7 +3722,7 @@
         <v>0.77814416594437008</v>
       </c>
     </row>
-    <row r="199" spans="1:3">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A199" s="1" t="s">
         <v>50</v>
       </c>
@@ -3826,7 +3733,7 @@
         <v>0.77786161563312584</v>
       </c>
     </row>
-    <row r="200" spans="1:3">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A200" s="1" t="s">
         <v>4</v>
       </c>
@@ -3837,7 +3744,7 @@
         <v>0.77760080356157901</v>
       </c>
     </row>
-    <row r="201" spans="1:3">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A201" s="1" t="s">
         <v>201</v>
       </c>
@@ -3848,7 +3755,7 @@
         <v>0.77736485005121747</v>
       </c>
     </row>
-    <row r="202" spans="1:3">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A202" s="1" t="s">
         <v>189</v>
       </c>
@@ -3859,7 +3766,7 @@
         <v>0.77715687542352851</v>
       </c>
     </row>
-    <row r="203" spans="1:3">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A203" s="1" t="s">
         <v>194</v>
       </c>
@@ -3870,7 +3777,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="204" spans="1:3">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A204" s="1" t="s">
         <v>14</v>
       </c>
@@ -3881,7 +3788,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="205" spans="1:3">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A205" s="1" t="s">
         <v>8</v>
       </c>
@@ -3892,7 +3799,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="206" spans="1:3">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A206" s="1" t="s">
         <v>7</v>
       </c>
@@ -3903,7 +3810,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="207" spans="1:3">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A207" s="1" t="s">
         <v>12</v>
       </c>
@@ -3914,7 +3821,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="208" spans="1:3">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A208" s="1" t="s">
         <v>13</v>
       </c>
@@ -3925,7 +3832,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="209" spans="1:3">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A209" s="1" t="s">
         <v>188</v>
       </c>
@@ -3936,7 +3843,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="210" spans="1:3">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A210" s="1" t="s">
         <v>196</v>
       </c>
@@ -3947,7 +3854,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="211" spans="1:3">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A211" s="1" t="s">
         <v>2</v>
       </c>
@@ -3958,7 +3865,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="212" spans="1:3">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A212" s="1" t="s">
         <v>191</v>
       </c>
@@ -3969,7 +3876,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="213" spans="1:3">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A213" s="1" t="s">
         <v>187</v>
       </c>
@@ -3980,7 +3887,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="214" spans="1:3">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A214" s="1" t="s">
         <v>1</v>
       </c>
@@ -3991,7 +3898,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="215" spans="1:3">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A215" s="1" t="s">
         <v>3</v>
       </c>
@@ -4002,7 +3909,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="216" spans="1:3">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A216" s="1" t="s">
         <v>55</v>
       </c>
@@ -4013,7 +3920,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="217" spans="1:3">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A217" s="1" t="s">
         <v>57</v>
       </c>
@@ -4024,7 +3931,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="218" spans="1:3">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A218" s="1" t="s">
         <v>11</v>
       </c>
@@ -4035,7 +3942,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="219" spans="1:3">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A219" s="1" t="s">
         <v>9</v>
       </c>
@@ -4046,7 +3953,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="220" spans="1:3">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A220" s="1" t="s">
         <v>47</v>
       </c>
@@ -4057,7 +3964,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="221" spans="1:3">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A221" s="1" t="s">
         <v>60</v>
       </c>
@@ -4068,7 +3975,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="222" spans="1:3">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A222" s="1" t="s">
         <v>10</v>
       </c>
@@ -4079,7 +3986,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="223" spans="1:3">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A223" s="1" t="s">
         <v>52</v>
       </c>
@@ -4090,7 +3997,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="224" spans="1:3">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A224" s="1" t="s">
         <v>59</v>
       </c>
@@ -4101,7 +4008,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="225" spans="1:3">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A225" s="1" t="s">
         <v>49</v>
       </c>
@@ -4112,7 +4019,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="226" spans="1:3">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A226" s="1" t="s">
         <v>48</v>
       </c>
@@ -4123,7 +4030,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="227" spans="1:3">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A227" s="1" t="s">
         <v>5</v>
       </c>
@@ -4134,7 +4041,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="228" spans="1:3">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A228" s="1" t="s">
         <v>6</v>
       </c>
@@ -4145,7 +4052,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="229" spans="1:3">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A229" s="1" t="s">
         <v>203</v>
       </c>
@@ -4156,7 +4063,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="230" spans="1:3">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A230" s="3" t="s">
         <v>231</v>
       </c>
@@ -4167,7 +4074,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="231" spans="1:3">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A231" s="3" t="s">
         <v>232</v>
       </c>
@@ -4178,7 +4085,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="232" spans="1:3">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A232" s="3" t="s">
         <v>233</v>
       </c>
@@ -4189,7 +4096,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="233" spans="1:3">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A233" s="3" t="s">
         <v>234</v>
       </c>
@@ -4200,7 +4107,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="234" spans="1:3">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A234" s="3" t="s">
         <v>235</v>
       </c>
@@ -4211,7 +4118,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="235" spans="1:3">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A235" s="3" t="s">
         <v>236</v>
       </c>
@@ -4222,7 +4129,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="236" spans="1:3">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A236" s="3" t="s">
         <v>237</v>
       </c>
@@ -4233,7 +4140,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="237" spans="1:3">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A237" s="3" t="s">
         <v>238</v>
       </c>
@@ -4244,7 +4151,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="238" spans="1:3">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A238" s="3" t="s">
         <v>239</v>
       </c>
@@ -4255,7 +4162,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="239" spans="1:3">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A239" s="3" t="s">
         <v>240</v>
       </c>
@@ -4266,7 +4173,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="240" spans="1:3">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A240" s="3" t="s">
         <v>241</v>
       </c>
@@ -4277,7 +4184,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="241" spans="1:3">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A241" s="3" t="s">
         <v>242</v>
       </c>
@@ -4288,7 +4195,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="242" spans="1:3">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A242" s="3" t="s">
         <v>243</v>
       </c>
@@ -4299,7 +4206,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="243" spans="1:3">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A243" s="3" t="s">
         <v>244</v>
       </c>
@@ -4310,7 +4217,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="244" spans="1:3">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A244" s="3" t="s">
         <v>245</v>
       </c>
@@ -4321,7 +4228,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="245" spans="1:3">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A245" s="3" t="s">
         <v>246</v>
       </c>
@@ -4332,7 +4239,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="246" spans="1:3">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A246" s="3" t="s">
         <v>247</v>
       </c>
@@ -4343,7 +4250,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="247" spans="1:3">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A247" s="3" t="s">
         <v>248</v>
       </c>
@@ -4354,7 +4261,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="248" spans="1:3">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A248" s="3" t="s">
         <v>249</v>
       </c>
@@ -4365,7 +4272,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="249" spans="1:3">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A249" s="3" t="s">
         <v>250</v>
       </c>
@@ -4376,7 +4283,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="250" spans="1:3">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A250" s="3" t="s">
         <v>251</v>
       </c>
@@ -4387,7 +4294,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="251" spans="1:3">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A251" s="3" t="s">
         <v>252</v>
       </c>
@@ -4398,7 +4305,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="252" spans="1:3">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A252" s="3" t="s">
         <v>253</v>
       </c>
@@ -4409,7 +4316,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="253" spans="1:3">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A253" s="3" t="s">
         <v>254</v>
       </c>
@@ -4420,7 +4327,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="254" spans="1:3">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A254" s="3" t="s">
         <v>255</v>
       </c>
@@ -4431,7 +4338,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="255" spans="1:3">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A255" s="3" t="s">
         <v>256</v>
       </c>
@@ -4442,7 +4349,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="256" spans="1:3">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A256" s="3" t="s">
         <v>257</v>
       </c>
@@ -4453,7 +4360,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="257" spans="1:3">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A257" s="3" t="s">
         <v>258</v>
       </c>
@@ -4464,7 +4371,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="258" spans="1:3">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A258" s="3" t="s">
         <v>259</v>
       </c>
@@ -4475,7 +4382,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="259" spans="1:3">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A259" s="3" t="s">
         <v>260</v>
       </c>
@@ -4486,7 +4393,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="260" spans="1:3">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A260" s="3" t="s">
         <v>261</v>
       </c>
@@ -4497,7 +4404,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="261" spans="1:3">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A261" s="3" t="s">
         <v>262</v>
       </c>
@@ -4508,7 +4415,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="262" spans="1:3">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A262" s="3" t="s">
         <v>263</v>
       </c>
@@ -4519,7 +4426,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="263" spans="1:3">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A263" s="3" t="s">
         <v>264</v>
       </c>
@@ -4530,7 +4437,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="264" spans="1:3">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A264" s="3" t="s">
         <v>265</v>
       </c>
@@ -4541,7 +4448,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="265" spans="1:3">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A265" s="3" t="s">
         <v>266</v>
       </c>
@@ -4552,7 +4459,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="266" spans="1:3">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A266" s="3" t="s">
         <v>267</v>
       </c>
@@ -4563,7 +4470,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="267" spans="1:3">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A267" s="3" t="s">
         <v>268</v>
       </c>
@@ -4574,7 +4481,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="268" spans="1:3">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A268" s="3" t="s">
         <v>269</v>
       </c>
@@ -4585,7 +4492,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="269" spans="1:3">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A269" s="3" t="s">
         <v>270</v>
       </c>
@@ -4596,7 +4503,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="270" spans="1:3">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A270" s="3" t="s">
         <v>271</v>
       </c>
@@ -4607,7 +4514,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="271" spans="1:3">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A271" s="3" t="s">
         <v>272</v>
       </c>
@@ -4618,7 +4525,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="272" spans="1:3">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A272" s="3" t="s">
         <v>273</v>
       </c>
@@ -4629,7 +4536,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="273" spans="1:3">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A273" s="3" t="s">
         <v>274</v>
       </c>
@@ -4640,7 +4547,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="274" spans="1:3">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A274" s="3" t="s">
         <v>275</v>
       </c>
@@ -4651,7 +4558,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="275" spans="1:3">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A275" s="3" t="s">
         <v>276</v>
       </c>
@@ -4662,7 +4569,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="276" spans="1:3">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A276" s="3" t="s">
         <v>277</v>
       </c>
@@ -4673,7 +4580,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="277" spans="1:3">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A277" s="3" t="s">
         <v>278</v>
       </c>
@@ -4684,7 +4591,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="278" spans="1:3">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A278" s="3" t="s">
         <v>279</v>
       </c>
@@ -4695,7 +4602,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="279" spans="1:3">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A279" s="3" t="s">
         <v>280</v>
       </c>
@@ -4706,7 +4613,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="280" spans="1:3">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A280" s="3" t="s">
         <v>281</v>
       </c>
@@ -4717,7 +4624,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="281" spans="1:3">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A281" s="3" t="s">
         <v>282</v>
       </c>
@@ -4728,7 +4635,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="282" spans="1:3">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A282" s="3" t="s">
         <v>283</v>
       </c>
@@ -4739,7 +4646,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="283" spans="1:3">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A283" s="3" t="s">
         <v>284</v>
       </c>
@@ -4750,7 +4657,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="284" spans="1:3">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A284" s="3" t="s">
         <v>285</v>
       </c>
@@ -4761,7 +4668,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="285" spans="1:3">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A285" s="3" t="s">
         <v>286</v>
       </c>
@@ -4772,7 +4679,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="286" spans="1:3">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A286" s="3" t="s">
         <v>287</v>
       </c>
@@ -4783,7 +4690,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="287" spans="1:3">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A287" s="3" t="s">
         <v>288</v>
       </c>
@@ -4794,7 +4701,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="288" spans="1:3">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A288" s="3" t="s">
         <v>289</v>
       </c>
@@ -4805,7 +4712,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="289" spans="1:3">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A289" s="3" t="s">
         <v>290</v>
       </c>
@@ -4816,7 +4723,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="290" spans="1:3">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A290" s="3" t="s">
         <v>291</v>
       </c>
@@ -4827,7 +4734,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="291" spans="1:3">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A291" s="3" t="s">
         <v>292</v>
       </c>
@@ -4838,7 +4745,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="292" spans="1:3">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A292" s="3" t="s">
         <v>293</v>
       </c>
@@ -4849,7 +4756,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="293" spans="1:3">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A293" s="3" t="s">
         <v>294</v>
       </c>
@@ -4860,7 +4767,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="294" spans="1:3">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A294" s="3" t="s">
         <v>295</v>
       </c>
@@ -4871,7 +4778,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="295" spans="1:3">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A295" s="3" t="s">
         <v>296</v>
       </c>
@@ -4882,7 +4789,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="296" spans="1:3">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A296" s="3" t="s">
         <v>297</v>
       </c>
@@ -4893,7 +4800,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="297" spans="1:3">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A297" s="3" t="s">
         <v>298</v>
       </c>
@@ -4904,7 +4811,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="298" spans="1:3">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A298" s="3" t="s">
         <v>299</v>
       </c>
@@ -4915,7 +4822,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="299" spans="1:3">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A299" s="3" t="s">
         <v>300</v>
       </c>
@@ -4926,7 +4833,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="300" spans="1:3">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A300" s="3" t="s">
         <v>301</v>
       </c>
@@ -4937,7 +4844,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="301" spans="1:3">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A301" s="3" t="s">
         <v>302</v>
       </c>
@@ -4948,7 +4855,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="302" spans="1:3">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A302" s="3" t="s">
         <v>303</v>
       </c>
@@ -4959,7 +4866,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="303" spans="1:3">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A303" s="3" t="s">
         <v>304</v>
       </c>
@@ -4970,7 +4877,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="304" spans="1:3">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A304" s="3" t="s">
         <v>305</v>
       </c>
@@ -4981,7 +4888,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="305" spans="1:3">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A305" s="3" t="s">
         <v>306</v>
       </c>
@@ -4992,7 +4899,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="306" spans="1:3">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A306" s="3" t="s">
         <v>307</v>
       </c>
@@ -5003,7 +4910,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="307" spans="1:3">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A307" s="3" t="s">
         <v>308</v>
       </c>
@@ -5014,7 +4921,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="308" spans="1:3">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A308" s="3" t="s">
         <v>309</v>
       </c>
@@ -5025,7 +4932,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="309" spans="1:3">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A309" s="3" t="s">
         <v>310</v>
       </c>
@@ -5036,7 +4943,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="310" spans="1:3">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A310" s="3" t="s">
         <v>311</v>
       </c>
@@ -5047,7 +4954,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="311" spans="1:3">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A311" s="3" t="s">
         <v>312</v>
       </c>
@@ -5058,7 +4965,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="312" spans="1:3">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A312" s="3" t="s">
         <v>313</v>
       </c>
@@ -5069,7 +4976,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="313" spans="1:3">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A313" s="3" t="s">
         <v>314</v>
       </c>
@@ -5080,7 +4987,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="314" spans="1:3">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A314" s="3" t="s">
         <v>315</v>
       </c>
@@ -5091,7 +4998,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="315" spans="1:3">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A315" s="3" t="s">
         <v>316</v>
       </c>
@@ -5102,7 +5009,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="316" spans="1:3">
+    <row r="316" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A316" s="3" t="s">
         <v>317</v>
       </c>
@@ -5113,7 +5020,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="317" spans="1:3">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A317" s="3" t="s">
         <v>318</v>
       </c>
@@ -5124,7 +5031,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="318" spans="1:3">
+    <row r="318" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A318" s="3" t="s">
         <v>319</v>
       </c>
@@ -5135,7 +5042,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="319" spans="1:3">
+    <row r="319" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A319" s="3" t="s">
         <v>320</v>
       </c>
@@ -5146,7 +5053,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="320" spans="1:3">
+    <row r="320" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A320" s="3" t="s">
         <v>321</v>
       </c>
@@ -5157,7 +5064,7 @@
         <v>0.77698</v>
       </c>
     </row>
-    <row r="321" spans="1:3">
+    <row r="321" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A321" s="3" t="s">
         <v>322</v>
       </c>
@@ -5165,347 +5072,6 @@
         <v>0.33258999999999994</v>
       </c>
       <c r="C321" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="322" spans="1:3">
-      <c r="A322" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="B322" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C322" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="323" spans="1:3">
-      <c r="A323" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="B323" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C323" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="324" spans="1:3">
-      <c r="A324" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="B324" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C324" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="325" spans="1:3">
-      <c r="A325" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="B325" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C325" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="326" spans="1:3">
-      <c r="A326" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="B326" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C326" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="327" spans="1:3">
-      <c r="A327" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="B327" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C327" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="328" spans="1:3">
-      <c r="A328" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="B328" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C328" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="329" spans="1:3">
-      <c r="A329" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="B329" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C329" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="330" spans="1:3">
-      <c r="A330" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="B330" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C330" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="331" spans="1:3">
-      <c r="A331" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="B331" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C331" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="332" spans="1:3">
-      <c r="A332" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="B332" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C332" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="333" spans="1:3">
-      <c r="A333" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="B333" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C333" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="334" spans="1:3">
-      <c r="A334" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="B334" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C334" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="335" spans="1:3">
-      <c r="A335" s="3" t="s">
-        <v>336</v>
-      </c>
-      <c r="B335" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C335" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="336" spans="1:3">
-      <c r="A336" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="B336" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C336" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="337" spans="1:3">
-      <c r="A337" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="B337" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C337" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="338" spans="1:3">
-      <c r="A338" s="3" t="s">
-        <v>339</v>
-      </c>
-      <c r="B338" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C338" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="339" spans="1:3">
-      <c r="A339" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="B339" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C339" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="340" spans="1:3">
-      <c r="A340" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="B340" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C340" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="341" spans="1:3">
-      <c r="A341" s="3" t="s">
-        <v>342</v>
-      </c>
-      <c r="B341" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C341" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="342" spans="1:3">
-      <c r="A342" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="B342" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C342" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="343" spans="1:3">
-      <c r="A343" s="3" t="s">
-        <v>344</v>
-      </c>
-      <c r="B343" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C343" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="344" spans="1:3">
-      <c r="A344" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="B344" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C344" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="345" spans="1:3">
-      <c r="A345" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="B345" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C345" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="346" spans="1:3">
-      <c r="A346" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="B346" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C346" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="347" spans="1:3">
-      <c r="A347" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="B347" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C347" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="348" spans="1:3">
-      <c r="A348" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="B348" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C348" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="349" spans="1:3">
-      <c r="A349" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="B349" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C349" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="350" spans="1:3">
-      <c r="A350" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="B350" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C350" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="351" spans="1:3">
-      <c r="A351" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="B351" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C351" s="1">
-        <v>0.77698</v>
-      </c>
-    </row>
-    <row r="352" spans="1:3">
-      <c r="A352" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="B352" s="1">
-        <v>0.33258999999999994</v>
-      </c>
-      <c r="C352" s="1">
         <v>0.77698</v>
       </c>
     </row>

</xml_diff>